<commit_message>
Fixed bug in v1 of ARO. Added code for v2. Added ARO historic for versions
</commit_message>
<xml_diff>
--- a/cec2017real-master/code/results_ARO/results_cec2017_10.xlsx
+++ b/cec2017real-master/code/results_ARO/results_cec2017_10.xlsx
@@ -603,94 +603,94 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>1548451000</v>
+        <v>1030591825</v>
       </c>
       <c r="D2" t="n">
-        <v>9181419000</v>
+        <v>3235295801.666667</v>
       </c>
       <c r="E2" t="n">
-        <v>17554.45</v>
+        <v>20354.88666666667</v>
       </c>
       <c r="F2" t="n">
-        <v>73.87062</v>
+        <v>80.16824333333334</v>
       </c>
       <c r="G2" t="n">
-        <v>67.33969999999999</v>
+        <v>65.14637666666665</v>
       </c>
       <c r="H2" t="n">
-        <v>29.63963</v>
+        <v>33.17864333333333</v>
       </c>
       <c r="I2" t="n">
-        <v>134.6132</v>
+        <v>125.9614666666667</v>
       </c>
       <c r="J2" t="n">
-        <v>78.41227000000001</v>
+        <v>75.20784666666667</v>
       </c>
       <c r="K2" t="n">
-        <v>337.9431</v>
+        <v>378.2727333333333</v>
       </c>
       <c r="L2" t="n">
-        <v>2016.304</v>
+        <v>1902.217333333333</v>
       </c>
       <c r="M2" t="n">
-        <v>985.4792</v>
+        <v>417.7382666666667</v>
       </c>
       <c r="N2" t="n">
-        <v>79396300</v>
+        <v>39261890</v>
       </c>
       <c r="O2" t="n">
-        <v>1187944</v>
+        <v>438304.9666666666</v>
       </c>
       <c r="P2" t="n">
-        <v>3142.241</v>
+        <v>8746.462333333335</v>
       </c>
       <c r="Q2" t="n">
-        <v>27639.43</v>
+        <v>11582.477</v>
       </c>
       <c r="R2" t="n">
-        <v>560.4627</v>
+        <v>388.4629333333334</v>
       </c>
       <c r="S2" t="n">
-        <v>270.4331</v>
+        <v>198.1231666666667</v>
       </c>
       <c r="T2" t="n">
-        <v>2415829</v>
+        <v>1027310.566666667</v>
       </c>
       <c r="U2" t="n">
-        <v>34112.68</v>
+        <v>37384.87666666667</v>
       </c>
       <c r="V2" t="n">
-        <v>399.5037</v>
+        <v>335.3313</v>
       </c>
       <c r="W2" t="n">
-        <v>278.1074</v>
+        <v>269.8901</v>
       </c>
       <c r="X2" t="n">
-        <v>2297.96</v>
+        <v>882.5045333333334</v>
       </c>
       <c r="Y2" t="n">
-        <v>371.4647</v>
+        <v>363.2805333333333</v>
       </c>
       <c r="Z2" t="n">
-        <v>400.385</v>
+        <v>397.8634666666667</v>
       </c>
       <c r="AA2" t="n">
-        <v>502.9439</v>
+        <v>485.5490666666666</v>
       </c>
       <c r="AB2" t="n">
-        <v>1367.267</v>
+        <v>1174.1834</v>
       </c>
       <c r="AC2" t="n">
-        <v>406.5506</v>
+        <v>403.488</v>
       </c>
       <c r="AD2" t="n">
-        <v>593.433</v>
+        <v>564.1365333333333</v>
       </c>
       <c r="AE2" t="n">
-        <v>613.3799</v>
+        <v>553.4175</v>
       </c>
       <c r="AF2" t="n">
-        <v>6224590</v>
+        <v>8816715.666666666</v>
       </c>
       <c r="AG2" t="n">
         <v>10</v>
@@ -704,94 +704,94 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>1548451000</v>
+        <v>946118150</v>
       </c>
       <c r="D3" t="n">
-        <v>2362004000</v>
+        <v>960203271</v>
       </c>
       <c r="E3" t="n">
-        <v>7247.667</v>
+        <v>11604.33133333333</v>
       </c>
       <c r="F3" t="n">
-        <v>64.4701</v>
+        <v>61.88990999999999</v>
       </c>
       <c r="G3" t="n">
-        <v>58.44707</v>
+        <v>62.18216666666666</v>
       </c>
       <c r="H3" t="n">
-        <v>20.06089</v>
+        <v>21.56056</v>
       </c>
       <c r="I3" t="n">
-        <v>134.6132</v>
+        <v>113.3810066666667</v>
       </c>
       <c r="J3" t="n">
-        <v>68.10579</v>
+        <v>68.31301333333333</v>
       </c>
       <c r="K3" t="n">
-        <v>337.9431</v>
+        <v>215.2853</v>
       </c>
       <c r="L3" t="n">
-        <v>1990.647</v>
+        <v>1893.665</v>
       </c>
       <c r="M3" t="n">
-        <v>571.4532</v>
+        <v>248.6389333333334</v>
       </c>
       <c r="N3" t="n">
-        <v>46254800</v>
+        <v>27960256.66666667</v>
       </c>
       <c r="O3" t="n">
-        <v>323676.8</v>
+        <v>146536.2466666667</v>
       </c>
       <c r="P3" t="n">
-        <v>3142.241</v>
+        <v>8487.012000000001</v>
       </c>
       <c r="Q3" t="n">
-        <v>21445.45</v>
+        <v>9430.586000000001</v>
       </c>
       <c r="R3" t="n">
-        <v>103.7797</v>
+        <v>235.2118666666667</v>
       </c>
       <c r="S3" t="n">
-        <v>217.0742</v>
+        <v>163.6866</v>
       </c>
       <c r="T3" t="n">
-        <v>593668.4</v>
+        <v>411796.6666666667</v>
       </c>
       <c r="U3" t="n">
-        <v>34112.68</v>
+        <v>19404.97066666666</v>
       </c>
       <c r="V3" t="n">
-        <v>182.1846</v>
+        <v>223.6242666666667</v>
       </c>
       <c r="W3" t="n">
-        <v>266.144</v>
+        <v>263.3021333333334</v>
       </c>
       <c r="X3" t="n">
-        <v>2162.146</v>
+        <v>827.5850666666666</v>
       </c>
       <c r="Y3" t="n">
-        <v>371.4647</v>
+        <v>354.9084333333333</v>
       </c>
       <c r="Z3" t="n">
-        <v>400.385</v>
+        <v>393.8506</v>
       </c>
       <c r="AA3" t="n">
-        <v>502.9439</v>
+        <v>478.6775666666667</v>
       </c>
       <c r="AB3" t="n">
-        <v>1004.137</v>
+        <v>1024.9634</v>
       </c>
       <c r="AC3" t="n">
-        <v>406.5506</v>
+        <v>401.4917</v>
       </c>
       <c r="AD3" t="n">
-        <v>593.433</v>
+        <v>562.9882</v>
       </c>
       <c r="AE3" t="n">
-        <v>613.3799</v>
+        <v>501.1417</v>
       </c>
       <c r="AF3" t="n">
-        <v>6224590</v>
+        <v>3670687.666666667</v>
       </c>
       <c r="AG3" t="n">
         <v>10</v>
@@ -805,94 +805,94 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>1548451000</v>
+        <v>925299150</v>
       </c>
       <c r="D4" t="n">
-        <v>75329830</v>
+        <v>59928277.66666666</v>
       </c>
       <c r="E4" t="n">
-        <v>7247.667</v>
+        <v>7087.860000000001</v>
       </c>
       <c r="F4" t="n">
-        <v>64.4701</v>
+        <v>54.53748</v>
       </c>
       <c r="G4" t="n">
-        <v>56.51869</v>
+        <v>61.49834333333333</v>
       </c>
       <c r="H4" t="n">
-        <v>20.06089</v>
+        <v>21.31247666666667</v>
       </c>
       <c r="I4" t="n">
-        <v>134.6132</v>
+        <v>113.3810066666667</v>
       </c>
       <c r="J4" t="n">
-        <v>68.10579</v>
+        <v>59.21405333333333</v>
       </c>
       <c r="K4" t="n">
-        <v>337.9431</v>
+        <v>215.2853</v>
       </c>
       <c r="L4" t="n">
-        <v>1990.647</v>
+        <v>1883.507</v>
       </c>
       <c r="M4" t="n">
-        <v>490.7304</v>
+        <v>218.3884266666666</v>
       </c>
       <c r="N4" t="n">
-        <v>46254800</v>
+        <v>24128720</v>
       </c>
       <c r="O4" t="n">
-        <v>323676.8</v>
+        <v>146505.4133333333</v>
       </c>
       <c r="P4" t="n">
-        <v>2390.067</v>
+        <v>6655.829999999999</v>
       </c>
       <c r="Q4" t="n">
-        <v>21445.45</v>
+        <v>9389.376</v>
       </c>
       <c r="R4" t="n">
-        <v>103.7797</v>
+        <v>192.6111</v>
       </c>
       <c r="S4" t="n">
-        <v>212.2861</v>
+        <v>162.0905666666667</v>
       </c>
       <c r="T4" t="n">
-        <v>414187.8</v>
+        <v>184429.7066666667</v>
       </c>
       <c r="U4" t="n">
-        <v>34112.68</v>
+        <v>16822.61266666667</v>
       </c>
       <c r="V4" t="n">
-        <v>164.3628</v>
+        <v>184.29558</v>
       </c>
       <c r="W4" t="n">
-        <v>252.1322</v>
+        <v>258.4595</v>
       </c>
       <c r="X4" t="n">
-        <v>2162.146</v>
+        <v>827.5850666666666</v>
       </c>
       <c r="Y4" t="n">
-        <v>360.7059</v>
+        <v>351.3221666666666</v>
       </c>
       <c r="Z4" t="n">
-        <v>389.0678</v>
+        <v>386.6436</v>
       </c>
       <c r="AA4" t="n">
-        <v>502.9439</v>
+        <v>478.6775666666667</v>
       </c>
       <c r="AB4" t="n">
-        <v>1004.137</v>
+        <v>980.3792</v>
       </c>
       <c r="AC4" t="n">
-        <v>406.5506</v>
+        <v>400.7378333333333</v>
       </c>
       <c r="AD4" t="n">
-        <v>591.2053</v>
+        <v>557.9956999999999</v>
       </c>
       <c r="AE4" t="n">
-        <v>613.3799</v>
+        <v>498.4493333333333</v>
       </c>
       <c r="AF4" t="n">
-        <v>5627146</v>
+        <v>3471539.666666667</v>
       </c>
       <c r="AG4" t="n">
         <v>10</v>
@@ -906,94 +906,94 @@
         <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>1548451000</v>
+        <v>922218075</v>
       </c>
       <c r="D5" t="n">
-        <v>37603180</v>
+        <v>43335704.66666666</v>
       </c>
       <c r="E5" t="n">
-        <v>4461.546</v>
+        <v>4901.726333333333</v>
       </c>
       <c r="F5" t="n">
-        <v>64.4701</v>
+        <v>50.47112333333333</v>
       </c>
       <c r="G5" t="n">
-        <v>56.51869</v>
+        <v>55.79481333333333</v>
       </c>
       <c r="H5" t="n">
-        <v>20.06089</v>
+        <v>18.59283333333333</v>
       </c>
       <c r="I5" t="n">
-        <v>134.6132</v>
+        <v>105.7552233333333</v>
       </c>
       <c r="J5" t="n">
-        <v>68.10579</v>
+        <v>57.16464</v>
       </c>
       <c r="K5" t="n">
-        <v>337.9431</v>
+        <v>209.7651666666667</v>
       </c>
       <c r="L5" t="n">
-        <v>1649.691</v>
+        <v>1686.595333333333</v>
       </c>
       <c r="M5" t="n">
-        <v>490.7304</v>
+        <v>217.3775833333333</v>
       </c>
       <c r="N5" t="n">
-        <v>19414270</v>
+        <v>15181876.66666667</v>
       </c>
       <c r="O5" t="n">
-        <v>323676.8</v>
+        <v>124959.3666666667</v>
       </c>
       <c r="P5" t="n">
-        <v>753.8679</v>
+        <v>4169.313966666667</v>
       </c>
       <c r="Q5" t="n">
-        <v>9270.023999999999</v>
+        <v>4889.600666666666</v>
       </c>
       <c r="R5" t="n">
-        <v>103.7797</v>
+        <v>191.6136666666666</v>
       </c>
       <c r="S5" t="n">
-        <v>189.6293</v>
+        <v>149.1698666666666</v>
       </c>
       <c r="T5" t="n">
-        <v>414187.8</v>
+        <v>173814.14</v>
       </c>
       <c r="U5" t="n">
-        <v>34112.68</v>
+        <v>16729.72766666667</v>
       </c>
       <c r="V5" t="n">
-        <v>164.3628</v>
+        <v>170.2606066666667</v>
       </c>
       <c r="W5" t="n">
-        <v>252.1322</v>
+        <v>254.7089666666667</v>
       </c>
       <c r="X5" t="n">
-        <v>2033.253</v>
+        <v>778.7688666666667</v>
       </c>
       <c r="Y5" t="n">
-        <v>360.7059</v>
+        <v>346.9702666666667</v>
       </c>
       <c r="Z5" t="n">
-        <v>378.097</v>
+        <v>376.6045666666666</v>
       </c>
       <c r="AA5" t="n">
-        <v>502.9439</v>
+        <v>472.9865</v>
       </c>
       <c r="AB5" t="n">
-        <v>951.9489</v>
+        <v>948.9504999999999</v>
       </c>
       <c r="AC5" t="n">
-        <v>406.5506</v>
+        <v>396.6344</v>
       </c>
       <c r="AD5" t="n">
-        <v>591.2053</v>
+        <v>557.7407333333333</v>
       </c>
       <c r="AE5" t="n">
-        <v>480.8104</v>
+        <v>405.5685666666666</v>
       </c>
       <c r="AF5" t="n">
-        <v>5627146</v>
+        <v>3317284.333333333</v>
       </c>
       <c r="AG5" t="n">
         <v>10</v>
@@ -1007,94 +1007,94 @@
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>1297893000</v>
+        <v>761708842.5</v>
       </c>
       <c r="D6" t="n">
-        <v>37603180</v>
+        <v>16465341.66666667</v>
       </c>
       <c r="E6" t="n">
-        <v>4461.546</v>
+        <v>3654.985666666667</v>
       </c>
       <c r="F6" t="n">
-        <v>51.31605</v>
+        <v>32.14791666666667</v>
       </c>
       <c r="G6" t="n">
-        <v>43.4102</v>
+        <v>47.70754333333334</v>
       </c>
       <c r="H6" t="n">
-        <v>20.06089</v>
+        <v>18.59283333333333</v>
       </c>
       <c r="I6" t="n">
-        <v>120.5847</v>
+        <v>98.52238999999999</v>
       </c>
       <c r="J6" t="n">
-        <v>63.79305</v>
+        <v>54.65403666666666</v>
       </c>
       <c r="K6" t="n">
-        <v>201.214</v>
+        <v>148.29924</v>
       </c>
       <c r="L6" t="n">
-        <v>1649.691</v>
+        <v>1651.515666666667</v>
       </c>
       <c r="M6" t="n">
-        <v>490.7304</v>
+        <v>208.5372933333333</v>
       </c>
       <c r="N6" t="n">
-        <v>19019460</v>
+        <v>12114964.66666667</v>
       </c>
       <c r="O6" t="n">
-        <v>323676.8</v>
+        <v>121718.9633333333</v>
       </c>
       <c r="P6" t="n">
-        <v>380.9496</v>
+        <v>307.1133333333333</v>
       </c>
       <c r="Q6" t="n">
-        <v>4665.203</v>
+        <v>2540.615666666667</v>
       </c>
       <c r="R6" t="n">
-        <v>103.7797</v>
+        <v>190.8993333333333</v>
       </c>
       <c r="S6" t="n">
-        <v>163.1145</v>
+        <v>132.8674</v>
       </c>
       <c r="T6" t="n">
-        <v>414187.8</v>
+        <v>163385.1733333333</v>
       </c>
       <c r="U6" t="n">
-        <v>8320.289000000001</v>
+        <v>5272.692333333333</v>
       </c>
       <c r="V6" t="n">
-        <v>142.6476</v>
+        <v>162.4625733333334</v>
       </c>
       <c r="W6" t="n">
-        <v>252.1322</v>
+        <v>253.4278</v>
       </c>
       <c r="X6" t="n">
-        <v>2033.253</v>
+        <v>771.0343333333334</v>
       </c>
       <c r="Y6" t="n">
-        <v>355.2404</v>
+        <v>344.5059333333334</v>
       </c>
       <c r="Z6" t="n">
-        <v>376.8496</v>
+        <v>376.1827</v>
       </c>
       <c r="AA6" t="n">
-        <v>502.9439</v>
+        <v>461.0725666666667</v>
       </c>
       <c r="AB6" t="n">
-        <v>951.9489</v>
+        <v>944.0127666666667</v>
       </c>
       <c r="AC6" t="n">
-        <v>403.9612</v>
+        <v>394.7369333333334</v>
       </c>
       <c r="AD6" t="n">
-        <v>591.2053</v>
+        <v>556.4135666666667</v>
       </c>
       <c r="AE6" t="n">
-        <v>461.538</v>
+        <v>396.0634333333333</v>
       </c>
       <c r="AF6" t="n">
-        <v>5627146</v>
+        <v>2547544.166666667</v>
       </c>
       <c r="AG6" t="n">
         <v>10</v>
@@ -1108,94 +1108,94 @@
         <v>20</v>
       </c>
       <c r="C7" t="n">
-        <v>988220400</v>
+        <v>603063827.5</v>
       </c>
       <c r="D7" t="n">
-        <v>37603180</v>
+        <v>12834534.33333333</v>
       </c>
       <c r="E7" t="n">
-        <v>2205.109</v>
+        <v>1933.912233333333</v>
       </c>
       <c r="F7" t="n">
-        <v>51.31605</v>
+        <v>25.06631333333333</v>
       </c>
       <c r="G7" t="n">
-        <v>43.4102</v>
+        <v>41.13237666666667</v>
       </c>
       <c r="H7" t="n">
-        <v>20.06089</v>
+        <v>18.080567</v>
       </c>
       <c r="I7" t="n">
-        <v>120.5847</v>
+        <v>92.85861999999999</v>
       </c>
       <c r="J7" t="n">
-        <v>58.77644</v>
+        <v>47.68894333333333</v>
       </c>
       <c r="K7" t="n">
-        <v>201.214</v>
+        <v>142.8669</v>
       </c>
       <c r="L7" t="n">
-        <v>1649.691</v>
+        <v>1527.833333333333</v>
       </c>
       <c r="M7" t="n">
-        <v>428.0975</v>
+        <v>186.40526</v>
       </c>
       <c r="N7" t="n">
-        <v>9802994</v>
+        <v>4770059.100000001</v>
       </c>
       <c r="O7" t="n">
-        <v>92057.64999999999</v>
+        <v>44505.39333333333</v>
       </c>
       <c r="P7" t="n">
-        <v>268.5325</v>
+        <v>225.5058</v>
       </c>
       <c r="Q7" t="n">
-        <v>2393.025</v>
+        <v>1061.910213333333</v>
       </c>
       <c r="R7" t="n">
-        <v>103.7797</v>
+        <v>186.4276</v>
       </c>
       <c r="S7" t="n">
-        <v>121.0738</v>
+        <v>82.89663333333333</v>
       </c>
       <c r="T7" t="n">
-        <v>90667.91</v>
+        <v>54725.78</v>
       </c>
       <c r="U7" t="n">
-        <v>8320.289000000001</v>
+        <v>3197.9913</v>
       </c>
       <c r="V7" t="n">
-        <v>72.78691999999999</v>
+        <v>134.8209366666667</v>
       </c>
       <c r="W7" t="n">
-        <v>252.1322</v>
+        <v>248.9355</v>
       </c>
       <c r="X7" t="n">
-        <v>1825.723</v>
+        <v>694.458</v>
       </c>
       <c r="Y7" t="n">
-        <v>350.5169</v>
+        <v>339.2614</v>
       </c>
       <c r="Z7" t="n">
-        <v>376.219</v>
+        <v>372.8585666666666</v>
       </c>
       <c r="AA7" t="n">
-        <v>502.9439</v>
+        <v>460.4704333333333</v>
       </c>
       <c r="AB7" t="n">
-        <v>933.0091</v>
+        <v>930.0726333333333</v>
       </c>
       <c r="AC7" t="n">
-        <v>403.3834</v>
+        <v>392.9822333333333</v>
       </c>
       <c r="AD7" t="n">
-        <v>484.1899</v>
+        <v>519.8583666666667</v>
       </c>
       <c r="AE7" t="n">
-        <v>461.538</v>
+        <v>384.1901333333333</v>
       </c>
       <c r="AF7" t="n">
-        <v>2842349</v>
+        <v>1280727.866666667</v>
       </c>
       <c r="AG7" t="n">
         <v>10</v>
@@ -1209,94 +1209,94 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>988220400</v>
+        <v>566648917.5</v>
       </c>
       <c r="D8" t="n">
-        <v>11100680</v>
+        <v>3931208</v>
       </c>
       <c r="E8" t="n">
-        <v>2205.109</v>
+        <v>1740.677033333333</v>
       </c>
       <c r="F8" t="n">
-        <v>51.31605</v>
+        <v>25.06631333333333</v>
       </c>
       <c r="G8" t="n">
-        <v>43.4102</v>
+        <v>35.70346666666666</v>
       </c>
       <c r="H8" t="n">
-        <v>19.70529</v>
+        <v>17.648793</v>
       </c>
       <c r="I8" t="n">
-        <v>114.6934</v>
+        <v>78.16088999999999</v>
       </c>
       <c r="J8" t="n">
-        <v>58.77644</v>
+        <v>46.69415666666666</v>
       </c>
       <c r="K8" t="n">
-        <v>201.214</v>
+        <v>120.84693</v>
       </c>
       <c r="L8" t="n">
-        <v>1649.691</v>
+        <v>1490.487666666667</v>
       </c>
       <c r="M8" t="n">
-        <v>428.0975</v>
+        <v>185.46121</v>
       </c>
       <c r="N8" t="n">
-        <v>9802994</v>
+        <v>4731998.566666666</v>
       </c>
       <c r="O8" t="n">
-        <v>92057.64999999999</v>
+        <v>44503.55666666666</v>
       </c>
       <c r="P8" t="n">
-        <v>96.80856</v>
+        <v>119.9076033333333</v>
       </c>
       <c r="Q8" t="n">
-        <v>2393.025</v>
+        <v>963.6284433333334</v>
       </c>
       <c r="R8" t="n">
-        <v>103.7797</v>
+        <v>183.5077</v>
       </c>
       <c r="S8" t="n">
-        <v>121.0738</v>
+        <v>82.89663333333333</v>
       </c>
       <c r="T8" t="n">
-        <v>54686.87</v>
+        <v>42674.46666666667</v>
       </c>
       <c r="U8" t="n">
-        <v>407.3266</v>
+        <v>509.7605</v>
       </c>
       <c r="V8" t="n">
-        <v>72.78691999999999</v>
+        <v>106.4136033333333</v>
       </c>
       <c r="W8" t="n">
-        <v>252.1322</v>
+        <v>247.1531333333333</v>
       </c>
       <c r="X8" t="n">
-        <v>1825.723</v>
+        <v>693.7094000000001</v>
       </c>
       <c r="Y8" t="n">
-        <v>347.6429</v>
+        <v>338.3034</v>
       </c>
       <c r="Z8" t="n">
-        <v>376.219</v>
+        <v>372.5463333333334</v>
       </c>
       <c r="AA8" t="n">
-        <v>474.2014</v>
+        <v>446.7449666666666</v>
       </c>
       <c r="AB8" t="n">
-        <v>747.1271</v>
+        <v>866.2063333333334</v>
       </c>
       <c r="AC8" t="n">
-        <v>400.2439</v>
+        <v>391.8569666666667</v>
       </c>
       <c r="AD8" t="n">
-        <v>444.8797</v>
+        <v>505.5689666666667</v>
       </c>
       <c r="AE8" t="n">
-        <v>413.8287</v>
+        <v>363.3962333333334</v>
       </c>
       <c r="AF8" t="n">
-        <v>2842349</v>
+        <v>1268200.353333333</v>
       </c>
       <c r="AG8" t="n">
         <v>10</v>
@@ -1310,94 +1310,94 @@
         <v>40</v>
       </c>
       <c r="C9" t="n">
-        <v>980223000</v>
+        <v>554812792.5</v>
       </c>
       <c r="D9" t="n">
-        <v>8426999</v>
+        <v>3038682</v>
       </c>
       <c r="E9" t="n">
-        <v>2205.109</v>
+        <v>1395.428366666667</v>
       </c>
       <c r="F9" t="n">
-        <v>34.81281</v>
+        <v>19.56523333333334</v>
       </c>
       <c r="G9" t="n">
-        <v>43.4102</v>
+        <v>34.12332666666666</v>
       </c>
       <c r="H9" t="n">
-        <v>16.95925</v>
+        <v>13.62654966666667</v>
       </c>
       <c r="I9" t="n">
-        <v>114.6934</v>
+        <v>78.16088999999999</v>
       </c>
       <c r="J9" t="n">
-        <v>45.73425</v>
+        <v>39.63919666666667</v>
       </c>
       <c r="K9" t="n">
-        <v>201.214</v>
+        <v>103.4865766666667</v>
       </c>
       <c r="L9" t="n">
-        <v>1649.691</v>
+        <v>1408.494666666667</v>
       </c>
       <c r="M9" t="n">
-        <v>373.8977</v>
+        <v>167.39461</v>
       </c>
       <c r="N9" t="n">
-        <v>8144008</v>
+        <v>3455834.233333333</v>
       </c>
       <c r="O9" t="n">
-        <v>92057.64999999999</v>
+        <v>44503.52666666666</v>
       </c>
       <c r="P9" t="n">
-        <v>96.80856</v>
+        <v>109.1254333333333</v>
       </c>
       <c r="Q9" t="n">
-        <v>2020.109</v>
+        <v>823.7237933333332</v>
       </c>
       <c r="R9" t="n">
-        <v>103.7797</v>
+        <v>178.2539333333333</v>
       </c>
       <c r="S9" t="n">
-        <v>121.0738</v>
+        <v>82.89663333333333</v>
       </c>
       <c r="T9" t="n">
-        <v>54686.87</v>
+        <v>42605.45333333333</v>
       </c>
       <c r="U9" t="n">
-        <v>407.3266</v>
+        <v>509.4332666666667</v>
       </c>
       <c r="V9" t="n">
-        <v>72.78691999999999</v>
+        <v>93.86183</v>
       </c>
       <c r="W9" t="n">
-        <v>252.1322</v>
+        <v>247.1531333333333</v>
       </c>
       <c r="X9" t="n">
-        <v>1785.721</v>
+        <v>676.3579333333333</v>
       </c>
       <c r="Y9" t="n">
-        <v>341.074</v>
+        <v>336.1137666666667</v>
       </c>
       <c r="Z9" t="n">
-        <v>376.219</v>
+        <v>371.7933333333334</v>
       </c>
       <c r="AA9" t="n">
-        <v>474.2014</v>
+        <v>446.7449666666666</v>
       </c>
       <c r="AB9" t="n">
-        <v>747.1271</v>
+        <v>857.4763333333334</v>
       </c>
       <c r="AC9" t="n">
-        <v>400.2439</v>
+        <v>391.6720666666667</v>
       </c>
       <c r="AD9" t="n">
-        <v>444.8797</v>
+        <v>505.4050333333333</v>
       </c>
       <c r="AE9" t="n">
-        <v>325.1624</v>
+        <v>325.9426333333333</v>
       </c>
       <c r="AF9" t="n">
-        <v>2842349</v>
+        <v>1160304.066666667</v>
       </c>
       <c r="AG9" t="n">
         <v>10</v>
@@ -1411,94 +1411,94 @@
         <v>50</v>
       </c>
       <c r="C10" t="n">
-        <v>825823300</v>
+        <v>472250792.5</v>
       </c>
       <c r="D10" t="n">
-        <v>7654991</v>
+        <v>2767487</v>
       </c>
       <c r="E10" t="n">
-        <v>2205.109</v>
+        <v>1261.433033333333</v>
       </c>
       <c r="F10" t="n">
-        <v>34.81281</v>
+        <v>19.56523333333334</v>
       </c>
       <c r="G10" t="n">
-        <v>43.4102</v>
+        <v>33.12309666666667</v>
       </c>
       <c r="H10" t="n">
-        <v>16.95925</v>
+        <v>12.46344966666667</v>
       </c>
       <c r="I10" t="n">
-        <v>100.1055</v>
+        <v>73.29825666666666</v>
       </c>
       <c r="J10" t="n">
-        <v>45.73425</v>
+        <v>38.57175666666667</v>
       </c>
       <c r="K10" t="n">
-        <v>201.214</v>
+        <v>97.13361333333334</v>
       </c>
       <c r="L10" t="n">
-        <v>1578.219</v>
+        <v>1316.139666666667</v>
       </c>
       <c r="M10" t="n">
-        <v>373.8977</v>
+        <v>159.86191</v>
       </c>
       <c r="N10" t="n">
-        <v>8144008</v>
+        <v>3455834.233333333</v>
       </c>
       <c r="O10" t="n">
-        <v>92057.64999999999</v>
+        <v>44503.52666666666</v>
       </c>
       <c r="P10" t="n">
-        <v>96.80856</v>
+        <v>91.27098666666666</v>
       </c>
       <c r="Q10" t="n">
-        <v>2020.109</v>
+        <v>762.89386</v>
       </c>
       <c r="R10" t="n">
-        <v>93.35380000000001</v>
+        <v>174.3449</v>
       </c>
       <c r="S10" t="n">
-        <v>87.82131</v>
+        <v>71.81247</v>
       </c>
       <c r="T10" t="n">
-        <v>54686.87</v>
+        <v>42444.84666666667</v>
       </c>
       <c r="U10" t="n">
-        <v>407.3266</v>
+        <v>509.1351666666666</v>
       </c>
       <c r="V10" t="n">
-        <v>72.78691999999999</v>
+        <v>92.17073000000001</v>
       </c>
       <c r="W10" t="n">
-        <v>252.1322</v>
+        <v>244.6634</v>
       </c>
       <c r="X10" t="n">
-        <v>1785.721</v>
+        <v>673.0713333333333</v>
       </c>
       <c r="Y10" t="n">
-        <v>340.553</v>
+        <v>335.1825666666667</v>
       </c>
       <c r="Z10" t="n">
-        <v>376.219</v>
+        <v>371.7933333333334</v>
       </c>
       <c r="AA10" t="n">
-        <v>474.2014</v>
+        <v>445.7316</v>
       </c>
       <c r="AB10" t="n">
-        <v>747.1271</v>
+        <v>857.4763333333334</v>
       </c>
       <c r="AC10" t="n">
-        <v>400.2439</v>
+        <v>391.6594333333333</v>
       </c>
       <c r="AD10" t="n">
-        <v>429.695</v>
+        <v>497.7466</v>
       </c>
       <c r="AE10" t="n">
-        <v>325.1624</v>
+        <v>319.0167</v>
       </c>
       <c r="AF10" t="n">
-        <v>2842349</v>
+        <v>1160158.706666667</v>
       </c>
       <c r="AG10" t="n">
         <v>10</v>
@@ -1512,94 +1512,94 @@
         <v>60</v>
       </c>
       <c r="C11" t="n">
-        <v>825823300</v>
+        <v>444551665</v>
       </c>
       <c r="D11" t="n">
-        <v>1955238</v>
+        <v>724615.6666666666</v>
       </c>
       <c r="E11" t="n">
-        <v>2205.109</v>
+        <v>1261.433033333333</v>
       </c>
       <c r="F11" t="n">
-        <v>34.81281</v>
+        <v>18.95103366666667</v>
       </c>
       <c r="G11" t="n">
-        <v>43.4102</v>
+        <v>33.12309666666667</v>
       </c>
       <c r="H11" t="n">
-        <v>16.95925</v>
+        <v>12.140534</v>
       </c>
       <c r="I11" t="n">
-        <v>82.31474</v>
+        <v>67.36800333333333</v>
       </c>
       <c r="J11" t="n">
-        <v>45.73425</v>
+        <v>37.95751333333333</v>
       </c>
       <c r="K11" t="n">
-        <v>201.214</v>
+        <v>95.79225333333333</v>
       </c>
       <c r="L11" t="n">
-        <v>1149.3</v>
+        <v>1010.460033333333</v>
       </c>
       <c r="M11" t="n">
-        <v>373.8977</v>
+        <v>159.8309633333333</v>
       </c>
       <c r="N11" t="n">
-        <v>8144008</v>
+        <v>3455834.233333333</v>
       </c>
       <c r="O11" t="n">
-        <v>92057.64999999999</v>
+        <v>44503.52666666666</v>
       </c>
       <c r="P11" t="n">
-        <v>96.80856</v>
+        <v>91.27098666666666</v>
       </c>
       <c r="Q11" t="n">
-        <v>2020.109</v>
+        <v>734.9086600000001</v>
       </c>
       <c r="R11" t="n">
-        <v>93.35380000000001</v>
+        <v>170.9307333333333</v>
       </c>
       <c r="S11" t="n">
-        <v>68.41509000000001</v>
+        <v>64.95195</v>
       </c>
       <c r="T11" t="n">
-        <v>54686.87</v>
+        <v>38178.27</v>
       </c>
       <c r="U11" t="n">
-        <v>407.3266</v>
+        <v>400.8187333333333</v>
       </c>
       <c r="V11" t="n">
-        <v>72.78691999999999</v>
+        <v>91.87766333333333</v>
       </c>
       <c r="W11" t="n">
-        <v>252.1322</v>
+        <v>239.8679333333333</v>
       </c>
       <c r="X11" t="n">
-        <v>1785.721</v>
+        <v>673.0713333333333</v>
       </c>
       <c r="Y11" t="n">
-        <v>340.553</v>
+        <v>334.5393</v>
       </c>
       <c r="Z11" t="n">
-        <v>376.219</v>
+        <v>367.5732666666667</v>
       </c>
       <c r="AA11" t="n">
-        <v>474.2014</v>
+        <v>445.7316</v>
       </c>
       <c r="AB11" t="n">
-        <v>654.3488</v>
+        <v>826.5502333333334</v>
       </c>
       <c r="AC11" t="n">
-        <v>398.2039</v>
+        <v>390.9794333333334</v>
       </c>
       <c r="AD11" t="n">
-        <v>429.695</v>
+        <v>497.693</v>
       </c>
       <c r="AE11" t="n">
-        <v>302.1133</v>
+        <v>305.803</v>
       </c>
       <c r="AF11" t="n">
-        <v>2160611</v>
+        <v>932912.7066666667</v>
       </c>
       <c r="AG11" t="n">
         <v>10</v>
@@ -1613,94 +1613,94 @@
         <v>70</v>
       </c>
       <c r="C12" t="n">
-        <v>825823300</v>
+        <v>444551665</v>
       </c>
       <c r="D12" t="n">
-        <v>1955238</v>
+        <v>724615.6666666666</v>
       </c>
       <c r="E12" t="n">
-        <v>2205.109</v>
+        <v>1227.7037</v>
       </c>
       <c r="F12" t="n">
-        <v>34.81281</v>
+        <v>18.95103366666667</v>
       </c>
       <c r="G12" t="n">
-        <v>43.4102</v>
+        <v>32.92989</v>
       </c>
       <c r="H12" t="n">
-        <v>16.95925</v>
+        <v>10.99044466666667</v>
       </c>
       <c r="I12" t="n">
-        <v>82.31474</v>
+        <v>67.36800333333333</v>
       </c>
       <c r="J12" t="n">
-        <v>45.73425</v>
+        <v>37.95751333333333</v>
       </c>
       <c r="K12" t="n">
-        <v>201.214</v>
+        <v>95.79225333333333</v>
       </c>
       <c r="L12" t="n">
-        <v>1149.3</v>
+        <v>1010.460033333333</v>
       </c>
       <c r="M12" t="n">
-        <v>373.8977</v>
+        <v>159.8309633333333</v>
       </c>
       <c r="N12" t="n">
-        <v>8144008</v>
+        <v>3455834.233333333</v>
       </c>
       <c r="O12" t="n">
-        <v>92057.64999999999</v>
+        <v>44503.52666666666</v>
       </c>
       <c r="P12" t="n">
-        <v>85.55824</v>
+        <v>87.52087999999999</v>
       </c>
       <c r="Q12" t="n">
-        <v>2020.109</v>
+        <v>734.09135</v>
       </c>
       <c r="R12" t="n">
-        <v>57.09534</v>
+        <v>158.8442466666667</v>
       </c>
       <c r="S12" t="n">
-        <v>68.41509000000001</v>
+        <v>64.95195</v>
       </c>
       <c r="T12" t="n">
-        <v>54686.87</v>
+        <v>38178.27</v>
       </c>
       <c r="U12" t="n">
-        <v>407.3266</v>
+        <v>321.3539666666666</v>
       </c>
       <c r="V12" t="n">
-        <v>72.78691999999999</v>
+        <v>91.87766333333333</v>
       </c>
       <c r="W12" t="n">
-        <v>251.6444</v>
+        <v>239.7053333333333</v>
       </c>
       <c r="X12" t="n">
-        <v>1785.721</v>
+        <v>673.0713333333333</v>
       </c>
       <c r="Y12" t="n">
-        <v>336.4369</v>
+        <v>333.1672666666666</v>
       </c>
       <c r="Z12" t="n">
-        <v>376.219</v>
+        <v>367.5732666666667</v>
       </c>
       <c r="AA12" t="n">
-        <v>460.8632</v>
+        <v>441.1143</v>
       </c>
       <c r="AB12" t="n">
-        <v>654.3488</v>
+        <v>826.5502333333334</v>
       </c>
       <c r="AC12" t="n">
-        <v>398.2039</v>
+        <v>390.9794333333334</v>
       </c>
       <c r="AD12" t="n">
-        <v>429.695</v>
+        <v>497.6824</v>
       </c>
       <c r="AE12" t="n">
-        <v>302.1133</v>
+        <v>304.4019333333333</v>
       </c>
       <c r="AF12" t="n">
-        <v>2160611</v>
+        <v>924238.59</v>
       </c>
       <c r="AG12" t="n">
         <v>10</v>
@@ -1714,94 +1714,94 @@
         <v>80</v>
       </c>
       <c r="C13" t="n">
-        <v>825823300</v>
+        <v>444551665</v>
       </c>
       <c r="D13" t="n">
-        <v>1955238</v>
+        <v>722675.6666666666</v>
       </c>
       <c r="E13" t="n">
-        <v>2205.109</v>
+        <v>1227.7037</v>
       </c>
       <c r="F13" t="n">
-        <v>34.81281</v>
+        <v>18.95103366666667</v>
       </c>
       <c r="G13" t="n">
-        <v>43.4102</v>
+        <v>32.92989</v>
       </c>
       <c r="H13" t="n">
-        <v>15.32049</v>
+        <v>10.44419133333333</v>
       </c>
       <c r="I13" t="n">
-        <v>82.31474</v>
+        <v>67.36800333333333</v>
       </c>
       <c r="J13" t="n">
-        <v>45.73425</v>
+        <v>36.70078</v>
       </c>
       <c r="K13" t="n">
-        <v>201.214</v>
+        <v>95.79225333333333</v>
       </c>
       <c r="L13" t="n">
-        <v>1149.3</v>
+        <v>1010.460033333333</v>
       </c>
       <c r="M13" t="n">
-        <v>373.8977</v>
+        <v>150.4825533333333</v>
       </c>
       <c r="N13" t="n">
-        <v>8144008</v>
+        <v>3380718.233333333</v>
       </c>
       <c r="O13" t="n">
-        <v>92057.64999999999</v>
+        <v>44502.68333333333</v>
       </c>
       <c r="P13" t="n">
-        <v>85.55824</v>
+        <v>70.00276333333333</v>
       </c>
       <c r="Q13" t="n">
-        <v>1856.925</v>
+        <v>678.1455533333333</v>
       </c>
       <c r="R13" t="n">
-        <v>57.09534</v>
+        <v>158.8442466666667</v>
       </c>
       <c r="S13" t="n">
-        <v>68.41509000000001</v>
+        <v>56.03356</v>
       </c>
       <c r="T13" t="n">
-        <v>54686.87</v>
+        <v>37691.09666666667</v>
       </c>
       <c r="U13" t="n">
-        <v>407.3266</v>
+        <v>321.3539666666666</v>
       </c>
       <c r="V13" t="n">
-        <v>72.78691999999999</v>
+        <v>86.70908000000001</v>
       </c>
       <c r="W13" t="n">
-        <v>244.431</v>
+        <v>237.3008666666667</v>
       </c>
       <c r="X13" t="n">
-        <v>1747.783</v>
+        <v>660.4253333333332</v>
       </c>
       <c r="Y13" t="n">
-        <v>336.4369</v>
+        <v>333.1672666666666</v>
       </c>
       <c r="Z13" t="n">
-        <v>376.219</v>
+        <v>367.5732666666667</v>
       </c>
       <c r="AA13" t="n">
-        <v>460.8632</v>
+        <v>441.1143</v>
       </c>
       <c r="AB13" t="n">
-        <v>654.3488</v>
+        <v>823.8107333333334</v>
       </c>
       <c r="AC13" t="n">
-        <v>398.2039</v>
+        <v>390.9794333333334</v>
       </c>
       <c r="AD13" t="n">
-        <v>429.695</v>
+        <v>497.5073666666667</v>
       </c>
       <c r="AE13" t="n">
-        <v>302.1133</v>
+        <v>297.9873</v>
       </c>
       <c r="AF13" t="n">
-        <v>2160611</v>
+        <v>924238.59</v>
       </c>
       <c r="AG13" t="n">
         <v>10</v>
@@ -1815,94 +1815,94 @@
         <v>90</v>
       </c>
       <c r="C14" t="n">
-        <v>530734900</v>
+        <v>297007465</v>
       </c>
       <c r="D14" t="n">
-        <v>1955238</v>
+        <v>699082</v>
       </c>
       <c r="E14" t="n">
-        <v>2205.109</v>
+        <v>1227.7037</v>
       </c>
       <c r="F14" t="n">
-        <v>34.81281</v>
+        <v>18.87817366666667</v>
       </c>
       <c r="G14" t="n">
-        <v>43.4102</v>
+        <v>32.92989</v>
       </c>
       <c r="H14" t="n">
-        <v>15.32049</v>
+        <v>10.44419133333333</v>
       </c>
       <c r="I14" t="n">
-        <v>82.31474</v>
+        <v>67.36800333333333</v>
       </c>
       <c r="J14" t="n">
-        <v>45.73425</v>
+        <v>36.70078</v>
       </c>
       <c r="K14" t="n">
-        <v>182.1487</v>
+        <v>89.08792999999999</v>
       </c>
       <c r="L14" t="n">
-        <v>1149.3</v>
+        <v>1010.460033333333</v>
       </c>
       <c r="M14" t="n">
-        <v>365.9101</v>
+        <v>147.82002</v>
       </c>
       <c r="N14" t="n">
-        <v>8144008</v>
+        <v>3380718.233333333</v>
       </c>
       <c r="O14" t="n">
-        <v>88936.31</v>
+        <v>43462.23666666666</v>
       </c>
       <c r="P14" t="n">
-        <v>85.55824</v>
+        <v>70.00276333333333</v>
       </c>
       <c r="Q14" t="n">
-        <v>1596.807</v>
+        <v>591.2696533333334</v>
       </c>
       <c r="R14" t="n">
-        <v>57.09534</v>
+        <v>158.8442466666667</v>
       </c>
       <c r="S14" t="n">
-        <v>68.41509000000001</v>
+        <v>51.74518666666668</v>
       </c>
       <c r="T14" t="n">
-        <v>43945.12</v>
+        <v>34105.43333333333</v>
       </c>
       <c r="U14" t="n">
-        <v>407.3266</v>
+        <v>302.2129666666667</v>
       </c>
       <c r="V14" t="n">
-        <v>72.78691999999999</v>
+        <v>51.29524333333333</v>
       </c>
       <c r="W14" t="n">
-        <v>244.431</v>
+        <v>236.3963666666667</v>
       </c>
       <c r="X14" t="n">
-        <v>1747.783</v>
+        <v>660.4253333333332</v>
       </c>
       <c r="Y14" t="n">
-        <v>336.4369</v>
+        <v>333.1672666666666</v>
       </c>
       <c r="Z14" t="n">
-        <v>374.0328</v>
+        <v>366.5188333333334</v>
       </c>
       <c r="AA14" t="n">
-        <v>460.8632</v>
+        <v>440.6991666666666</v>
       </c>
       <c r="AB14" t="n">
-        <v>648.0073</v>
+        <v>820.9157333333333</v>
       </c>
       <c r="AC14" t="n">
-        <v>398.2039</v>
+        <v>390.7537333333333</v>
       </c>
       <c r="AD14" t="n">
-        <v>429.695</v>
+        <v>497.4596999999999</v>
       </c>
       <c r="AE14" t="n">
-        <v>302.1133</v>
+        <v>297.9873</v>
       </c>
       <c r="AF14" t="n">
-        <v>2160611</v>
+        <v>924238.59</v>
       </c>
       <c r="AG14" t="n">
         <v>10</v>
@@ -1916,94 +1916,94 @@
         <v>100</v>
       </c>
       <c r="C15" t="n">
-        <v>530734900</v>
+        <v>297007465</v>
       </c>
       <c r="D15" t="n">
-        <v>1955238</v>
+        <v>698477.6666666666</v>
       </c>
       <c r="E15" t="n">
-        <v>2205.109</v>
+        <v>1160.7656</v>
       </c>
       <c r="F15" t="n">
-        <v>18.05636</v>
+        <v>13.29269033333333</v>
       </c>
       <c r="G15" t="n">
-        <v>34.07952</v>
+        <v>27.36746333333333</v>
       </c>
       <c r="H15" t="n">
-        <v>15.32049</v>
+        <v>10.44419133333333</v>
       </c>
       <c r="I15" t="n">
-        <v>82.31474</v>
+        <v>67.36800333333333</v>
       </c>
       <c r="J15" t="n">
-        <v>45.73425</v>
+        <v>36.70078</v>
       </c>
       <c r="K15" t="n">
-        <v>182.1487</v>
+        <v>89.08792999999999</v>
       </c>
       <c r="L15" t="n">
-        <v>1149.3</v>
+        <v>1010.460033333333</v>
       </c>
       <c r="M15" t="n">
-        <v>365.9101</v>
+        <v>147.82002</v>
       </c>
       <c r="N15" t="n">
-        <v>8144008</v>
+        <v>3377578.166666667</v>
       </c>
       <c r="O15" t="n">
-        <v>88936.31</v>
+        <v>43462.23666666666</v>
       </c>
       <c r="P15" t="n">
-        <v>85.55824</v>
+        <v>70.00276333333333</v>
       </c>
       <c r="Q15" t="n">
-        <v>1125.226</v>
+        <v>434.0759866666667</v>
       </c>
       <c r="R15" t="n">
-        <v>57.09534</v>
+        <v>158.8442466666667</v>
       </c>
       <c r="S15" t="n">
-        <v>68.41509000000001</v>
+        <v>51.42884666666667</v>
       </c>
       <c r="T15" t="n">
-        <v>39596.45</v>
+        <v>32653.90333333333</v>
       </c>
       <c r="U15" t="n">
-        <v>407.3266</v>
+        <v>297.9023</v>
       </c>
       <c r="V15" t="n">
-        <v>72.78691999999999</v>
+        <v>51.29524333333333</v>
       </c>
       <c r="W15" t="n">
-        <v>244.431</v>
+        <v>236.3963666666667</v>
       </c>
       <c r="X15" t="n">
-        <v>1747.783</v>
+        <v>660.4253333333332</v>
       </c>
       <c r="Y15" t="n">
-        <v>336.4369</v>
+        <v>331.9504666666667</v>
       </c>
       <c r="Z15" t="n">
-        <v>373.2594</v>
+        <v>362.6881333333333</v>
       </c>
       <c r="AA15" t="n">
-        <v>460.8632</v>
+        <v>440.0640333333333</v>
       </c>
       <c r="AB15" t="n">
-        <v>648.0073</v>
+        <v>820.9157333333333</v>
       </c>
       <c r="AC15" t="n">
-        <v>398.2039</v>
+        <v>390.6434333333333</v>
       </c>
       <c r="AD15" t="n">
-        <v>429.695</v>
+        <v>497.4596999999999</v>
       </c>
       <c r="AE15" t="n">
-        <v>302.1133</v>
+        <v>297.9873</v>
       </c>
       <c r="AF15" t="n">
-        <v>1487051</v>
+        <v>699718.59</v>
       </c>
       <c r="AG15" t="n">
         <v>10</v>

</xml_diff>

<commit_message>
Added code for v3 (arithmetic crossover)
</commit_message>
<xml_diff>
--- a/cec2017real-master/code/results_ARO/results_cec2017_10.xlsx
+++ b/cec2017real-master/code/results_ARO/results_cec2017_10.xlsx
@@ -603,94 +603,94 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>1030591825</v>
+        <v>826528306</v>
       </c>
       <c r="D2" t="n">
-        <v>3235295801.666667</v>
+        <v>2436064906.25</v>
       </c>
       <c r="E2" t="n">
-        <v>20354.88666666667</v>
+        <v>20770.0275</v>
       </c>
       <c r="F2" t="n">
-        <v>80.16824333333334</v>
+        <v>80.33364</v>
       </c>
       <c r="G2" t="n">
-        <v>65.14637666666665</v>
+        <v>60.7313275</v>
       </c>
       <c r="H2" t="n">
-        <v>33.17864333333333</v>
+        <v>46.733985</v>
       </c>
       <c r="I2" t="n">
-        <v>125.9614666666667</v>
+        <v>115.214485</v>
       </c>
       <c r="J2" t="n">
-        <v>75.20784666666667</v>
+        <v>71.5203475</v>
       </c>
       <c r="K2" t="n">
-        <v>378.2727333333333</v>
+        <v>291.243275</v>
       </c>
       <c r="L2" t="n">
-        <v>1902.217333333333</v>
+        <v>1660.363225</v>
       </c>
       <c r="M2" t="n">
-        <v>417.7382666666667</v>
+        <v>413.169575</v>
       </c>
       <c r="N2" t="n">
-        <v>39261890</v>
+        <v>30188255</v>
       </c>
       <c r="O2" t="n">
-        <v>438304.9666666666</v>
+        <v>334101.8875</v>
       </c>
       <c r="P2" t="n">
-        <v>8746.462333333335</v>
+        <v>6667.700750000001</v>
       </c>
       <c r="Q2" t="n">
-        <v>11582.477</v>
+        <v>57840.08275</v>
       </c>
       <c r="R2" t="n">
-        <v>388.4629333333334</v>
+        <v>373.939675</v>
       </c>
       <c r="S2" t="n">
-        <v>198.1231666666667</v>
+        <v>187.9202</v>
       </c>
       <c r="T2" t="n">
-        <v>1027310.566666667</v>
+        <v>778568.845</v>
       </c>
       <c r="U2" t="n">
-        <v>37384.87666666667</v>
+        <v>29524.58975</v>
       </c>
       <c r="V2" t="n">
-        <v>335.3313</v>
+        <v>338.500175</v>
       </c>
       <c r="W2" t="n">
-        <v>269.8901</v>
+        <v>264.00015</v>
       </c>
       <c r="X2" t="n">
-        <v>882.5045333333334</v>
+        <v>690.643375</v>
       </c>
       <c r="Y2" t="n">
-        <v>363.2805333333333</v>
+        <v>375.728575</v>
       </c>
       <c r="Z2" t="n">
-        <v>397.8634666666667</v>
+        <v>396.547875</v>
       </c>
       <c r="AA2" t="n">
-        <v>485.5490666666666</v>
+        <v>479.080325</v>
       </c>
       <c r="AB2" t="n">
-        <v>1174.1834</v>
+        <v>962.647425</v>
       </c>
       <c r="AC2" t="n">
-        <v>403.488</v>
+        <v>421.68175</v>
       </c>
       <c r="AD2" t="n">
-        <v>564.1365333333333</v>
+        <v>527.0715250000001</v>
       </c>
       <c r="AE2" t="n">
-        <v>553.4175</v>
+        <v>503.4609</v>
       </c>
       <c r="AF2" t="n">
-        <v>8816715.666666666</v>
+        <v>7249508</v>
       </c>
       <c r="AG2" t="n">
         <v>10</v>
@@ -704,94 +704,94 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>946118150</v>
+        <v>757792392.6</v>
       </c>
       <c r="D3" t="n">
-        <v>960203271</v>
+        <v>720558647.75</v>
       </c>
       <c r="E3" t="n">
-        <v>11604.33133333333</v>
+        <v>10756.402</v>
       </c>
       <c r="F3" t="n">
-        <v>61.88990999999999</v>
+        <v>64.9858825</v>
       </c>
       <c r="G3" t="n">
-        <v>62.18216666666666</v>
+        <v>56.8046525</v>
       </c>
       <c r="H3" t="n">
-        <v>21.56056</v>
+        <v>28.7369475</v>
       </c>
       <c r="I3" t="n">
-        <v>113.3810066666667</v>
+        <v>104.20841</v>
       </c>
       <c r="J3" t="n">
-        <v>68.31301333333333</v>
+        <v>63.0274475</v>
       </c>
       <c r="K3" t="n">
-        <v>215.2853</v>
+        <v>168.71062</v>
       </c>
       <c r="L3" t="n">
-        <v>1893.665</v>
+        <v>1616.336225</v>
       </c>
       <c r="M3" t="n">
-        <v>248.6389333333334</v>
+        <v>274.047025</v>
       </c>
       <c r="N3" t="n">
-        <v>27960256.66666667</v>
+        <v>21628805.75</v>
       </c>
       <c r="O3" t="n">
-        <v>146536.2466666667</v>
+        <v>112920.165</v>
       </c>
       <c r="P3" t="n">
-        <v>8487.012000000001</v>
+        <v>6437.650025000001</v>
       </c>
       <c r="Q3" t="n">
-        <v>9430.586000000001</v>
+        <v>30801.7995</v>
       </c>
       <c r="R3" t="n">
-        <v>235.2118666666667</v>
+        <v>252.9839</v>
       </c>
       <c r="S3" t="n">
-        <v>163.6866</v>
+        <v>161.324525</v>
       </c>
       <c r="T3" t="n">
-        <v>411796.6666666667</v>
+        <v>316436.29</v>
       </c>
       <c r="U3" t="n">
-        <v>19404.97066666666</v>
+        <v>16039.66025</v>
       </c>
       <c r="V3" t="n">
-        <v>223.6242666666667</v>
+        <v>252.97155</v>
       </c>
       <c r="W3" t="n">
-        <v>263.3021333333334</v>
+        <v>257.774825</v>
       </c>
       <c r="X3" t="n">
-        <v>827.5850666666666</v>
+        <v>648.4328250000001</v>
       </c>
       <c r="Y3" t="n">
-        <v>354.9084333333333</v>
+        <v>351.0404</v>
       </c>
       <c r="Z3" t="n">
-        <v>393.8506</v>
+        <v>391.21795</v>
       </c>
       <c r="AA3" t="n">
-        <v>478.6775666666667</v>
+        <v>472.19895</v>
       </c>
       <c r="AB3" t="n">
-        <v>1024.9634</v>
+        <v>847.669525</v>
       </c>
       <c r="AC3" t="n">
-        <v>401.4917</v>
+        <v>419.954475</v>
       </c>
       <c r="AD3" t="n">
-        <v>562.9882</v>
+        <v>519.567175</v>
       </c>
       <c r="AE3" t="n">
-        <v>501.1417</v>
+        <v>464.25405</v>
       </c>
       <c r="AF3" t="n">
-        <v>3670687.666666667</v>
+        <v>3312836.25</v>
       </c>
       <c r="AG3" t="n">
         <v>10</v>
@@ -805,94 +805,94 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>925299150</v>
+        <v>740643774.6</v>
       </c>
       <c r="D4" t="n">
-        <v>59928277.66666666</v>
+        <v>44948152.75</v>
       </c>
       <c r="E4" t="n">
-        <v>7087.860000000001</v>
+        <v>5890.3485</v>
       </c>
       <c r="F4" t="n">
-        <v>54.53748</v>
+        <v>59.387545</v>
       </c>
       <c r="G4" t="n">
-        <v>61.49834333333333</v>
+        <v>56.17666</v>
       </c>
       <c r="H4" t="n">
-        <v>21.31247666666667</v>
+        <v>25.88164</v>
       </c>
       <c r="I4" t="n">
-        <v>113.3810066666667</v>
+        <v>100.9850275</v>
       </c>
       <c r="J4" t="n">
-        <v>59.21405333333333</v>
+        <v>55.99485</v>
       </c>
       <c r="K4" t="n">
-        <v>215.2853</v>
+        <v>166.1480925</v>
       </c>
       <c r="L4" t="n">
-        <v>1883.507</v>
+        <v>1597.909325</v>
       </c>
       <c r="M4" t="n">
-        <v>218.3884266666666</v>
+        <v>248.195495</v>
       </c>
       <c r="N4" t="n">
-        <v>24128720</v>
+        <v>18751916.75</v>
       </c>
       <c r="O4" t="n">
-        <v>146505.4133333333</v>
+        <v>112897.04</v>
       </c>
       <c r="P4" t="n">
-        <v>6655.829999999999</v>
+        <v>5046.208575</v>
       </c>
       <c r="Q4" t="n">
-        <v>9389.376</v>
+        <v>22065.7595</v>
       </c>
       <c r="R4" t="n">
-        <v>192.6111</v>
+        <v>218.619525</v>
       </c>
       <c r="S4" t="n">
-        <v>162.0905666666667</v>
+        <v>160.1275</v>
       </c>
       <c r="T4" t="n">
-        <v>184429.7066666667</v>
+        <v>145911.07</v>
       </c>
       <c r="U4" t="n">
-        <v>16822.61266666667</v>
+        <v>14021.28</v>
       </c>
       <c r="V4" t="n">
-        <v>184.29558</v>
+        <v>187.01936</v>
       </c>
       <c r="W4" t="n">
-        <v>258.4595</v>
+        <v>254.039075</v>
       </c>
       <c r="X4" t="n">
-        <v>827.5850666666666</v>
+        <v>648.2886000000001</v>
       </c>
       <c r="Y4" t="n">
-        <v>351.3221666666666</v>
+        <v>347.241275</v>
       </c>
       <c r="Z4" t="n">
-        <v>386.6436</v>
+        <v>385.548375</v>
       </c>
       <c r="AA4" t="n">
-        <v>478.6775666666667</v>
+        <v>471.596925</v>
       </c>
       <c r="AB4" t="n">
-        <v>980.3792</v>
+        <v>812.737</v>
       </c>
       <c r="AC4" t="n">
-        <v>400.7378333333333</v>
+        <v>419.33375</v>
       </c>
       <c r="AD4" t="n">
-        <v>557.9956999999999</v>
+        <v>514.801325</v>
       </c>
       <c r="AE4" t="n">
-        <v>498.4493333333333</v>
+        <v>461.27145</v>
       </c>
       <c r="AF4" t="n">
-        <v>3471539.666666667</v>
+        <v>3155519</v>
       </c>
       <c r="AG4" t="n">
         <v>10</v>
@@ -906,94 +906,94 @@
         <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>922218075</v>
+        <v>738063492.6</v>
       </c>
       <c r="D5" t="n">
-        <v>43335704.66666666</v>
+        <v>32502751</v>
       </c>
       <c r="E5" t="n">
-        <v>4901.726333333333</v>
+        <v>3767.74895</v>
       </c>
       <c r="F5" t="n">
-        <v>50.47112333333333</v>
+        <v>56.1555025</v>
       </c>
       <c r="G5" t="n">
-        <v>55.79481333333333</v>
+        <v>51.7026425</v>
       </c>
       <c r="H5" t="n">
-        <v>18.59283333333333</v>
+        <v>23.6674925</v>
       </c>
       <c r="I5" t="n">
-        <v>105.7552233333333</v>
+        <v>92.75526499999999</v>
       </c>
       <c r="J5" t="n">
-        <v>57.16464</v>
+        <v>54.3618775</v>
       </c>
       <c r="K5" t="n">
-        <v>209.7651666666667</v>
+        <v>159.9836625</v>
       </c>
       <c r="L5" t="n">
-        <v>1686.595333333333</v>
+        <v>1447.1329</v>
       </c>
       <c r="M5" t="n">
-        <v>217.3775833333333</v>
+        <v>245.3338375</v>
       </c>
       <c r="N5" t="n">
-        <v>15181876.66666667</v>
+        <v>12024384</v>
       </c>
       <c r="O5" t="n">
-        <v>124959.3666666667</v>
+        <v>96622.72749999999</v>
       </c>
       <c r="P5" t="n">
-        <v>4169.313966666667</v>
+        <v>3178.52515</v>
       </c>
       <c r="Q5" t="n">
-        <v>4889.600666666666</v>
+        <v>10295.763</v>
       </c>
       <c r="R5" t="n">
-        <v>191.6136666666666</v>
+        <v>205.452325</v>
       </c>
       <c r="S5" t="n">
-        <v>149.1698666666666</v>
+        <v>149.6699</v>
       </c>
       <c r="T5" t="n">
-        <v>173814.14</v>
+        <v>137386.1625</v>
       </c>
       <c r="U5" t="n">
-        <v>16729.72766666667</v>
+        <v>13900.053</v>
       </c>
       <c r="V5" t="n">
-        <v>170.2606066666667</v>
+        <v>165.75138</v>
       </c>
       <c r="W5" t="n">
-        <v>254.7089666666667</v>
+        <v>251.1193</v>
       </c>
       <c r="X5" t="n">
-        <v>778.7688666666667</v>
+        <v>611.22965</v>
       </c>
       <c r="Y5" t="n">
-        <v>346.9702666666667</v>
+        <v>341.085775</v>
       </c>
       <c r="Z5" t="n">
-        <v>376.6045666666666</v>
+        <v>377.893475</v>
       </c>
       <c r="AA5" t="n">
-        <v>472.9865</v>
+        <v>467.09275</v>
       </c>
       <c r="AB5" t="n">
-        <v>948.9504999999999</v>
+        <v>787.524775</v>
       </c>
       <c r="AC5" t="n">
-        <v>396.6344</v>
+        <v>416.081525</v>
       </c>
       <c r="AD5" t="n">
-        <v>557.7407333333333</v>
+        <v>513.7828499999999</v>
       </c>
       <c r="AE5" t="n">
-        <v>405.5685666666666</v>
+        <v>391.27645</v>
       </c>
       <c r="AF5" t="n">
-        <v>3317284.333333333</v>
+        <v>2977958.5</v>
       </c>
       <c r="AG5" t="n">
         <v>10</v>
@@ -1007,94 +1007,94 @@
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>761708842.5</v>
+        <v>609518145.96</v>
       </c>
       <c r="D6" t="n">
-        <v>16465341.66666667</v>
+        <v>12349515.25</v>
       </c>
       <c r="E6" t="n">
-        <v>3654.985666666667</v>
+        <v>2744.3232725</v>
       </c>
       <c r="F6" t="n">
-        <v>32.14791666666667</v>
+        <v>42.3586925</v>
       </c>
       <c r="G6" t="n">
-        <v>47.70754333333334</v>
+        <v>45.3392275</v>
       </c>
       <c r="H6" t="n">
-        <v>18.59283333333333</v>
+        <v>23.4605825</v>
       </c>
       <c r="I6" t="n">
-        <v>98.52238999999999</v>
+        <v>84.65531</v>
       </c>
       <c r="J6" t="n">
-        <v>54.65403666666666</v>
+        <v>52.473335</v>
       </c>
       <c r="K6" t="n">
-        <v>148.29924</v>
+        <v>113.48621375</v>
       </c>
       <c r="L6" t="n">
-        <v>1651.515666666667</v>
+        <v>1417.09785</v>
       </c>
       <c r="M6" t="n">
-        <v>208.5372933333333</v>
+        <v>238.052645</v>
       </c>
       <c r="N6" t="n">
-        <v>12114964.66666667</v>
+        <v>9597429.75</v>
       </c>
       <c r="O6" t="n">
-        <v>121718.9633333333</v>
+        <v>94134.48</v>
       </c>
       <c r="P6" t="n">
-        <v>307.1133333333333</v>
+        <v>260.0064</v>
       </c>
       <c r="Q6" t="n">
-        <v>2540.615666666667</v>
+        <v>3584.96825</v>
       </c>
       <c r="R6" t="n">
-        <v>190.8993333333333</v>
+        <v>200.59105</v>
       </c>
       <c r="S6" t="n">
-        <v>132.8674</v>
+        <v>137.384225</v>
       </c>
       <c r="T6" t="n">
-        <v>163385.1733333333</v>
+        <v>129563.91</v>
       </c>
       <c r="U6" t="n">
-        <v>5272.692333333333</v>
+        <v>4161.1053</v>
       </c>
       <c r="V6" t="n">
-        <v>162.4625733333334</v>
+        <v>152.26303</v>
       </c>
       <c r="W6" t="n">
-        <v>253.4278</v>
+        <v>250.0349</v>
       </c>
       <c r="X6" t="n">
-        <v>771.0343333333334</v>
+        <v>604.6635</v>
       </c>
       <c r="Y6" t="n">
-        <v>344.5059333333334</v>
+        <v>338.322575</v>
       </c>
       <c r="Z6" t="n">
-        <v>376.1827</v>
+        <v>377.49375</v>
       </c>
       <c r="AA6" t="n">
-        <v>461.0725666666667</v>
+        <v>458.143875</v>
       </c>
       <c r="AB6" t="n">
-        <v>944.0127666666667</v>
+        <v>783.2268</v>
       </c>
       <c r="AC6" t="n">
-        <v>394.7369333333334</v>
+        <v>414.596</v>
       </c>
       <c r="AD6" t="n">
-        <v>556.4135666666667</v>
+        <v>510.93615</v>
       </c>
       <c r="AE6" t="n">
-        <v>396.0634333333333</v>
+        <v>378.43775</v>
       </c>
       <c r="AF6" t="n">
-        <v>2547544.166666667</v>
+        <v>2050010.3</v>
       </c>
       <c r="AG6" t="n">
         <v>10</v>
@@ -1108,94 +1108,94 @@
         <v>20</v>
       </c>
       <c r="C7" t="n">
-        <v>603063827.5</v>
+        <v>482485646.1</v>
       </c>
       <c r="D7" t="n">
-        <v>12834534.33333333</v>
+        <v>9625953</v>
       </c>
       <c r="E7" t="n">
-        <v>1933.912233333333</v>
+        <v>1451.4752995</v>
       </c>
       <c r="F7" t="n">
-        <v>25.06631333333333</v>
+        <v>36.97904</v>
       </c>
       <c r="G7" t="n">
-        <v>41.13237666666667</v>
+        <v>40.2909875</v>
       </c>
       <c r="H7" t="n">
-        <v>18.080567</v>
+        <v>22.71446275</v>
       </c>
       <c r="I7" t="n">
-        <v>92.85861999999999</v>
+        <v>79.7488225</v>
       </c>
       <c r="J7" t="n">
-        <v>47.68894333333333</v>
+        <v>47.2369225</v>
       </c>
       <c r="K7" t="n">
-        <v>142.8669</v>
+        <v>109.21415525</v>
       </c>
       <c r="L7" t="n">
-        <v>1527.833333333333</v>
+        <v>1323.46</v>
       </c>
       <c r="M7" t="n">
-        <v>186.40526</v>
+        <v>212.04367</v>
       </c>
       <c r="N7" t="n">
-        <v>4770059.100000001</v>
+        <v>4086986.325</v>
       </c>
       <c r="O7" t="n">
-        <v>44505.39333333333</v>
+        <v>36224.3025</v>
       </c>
       <c r="P7" t="n">
-        <v>225.5058</v>
+        <v>195.42065</v>
       </c>
       <c r="Q7" t="n">
-        <v>1061.910213333333</v>
+        <v>926.93751</v>
       </c>
       <c r="R7" t="n">
-        <v>186.4276</v>
+        <v>195.804625</v>
       </c>
       <c r="S7" t="n">
-        <v>82.89663333333333</v>
+        <v>99.87965</v>
       </c>
       <c r="T7" t="n">
-        <v>54725.78</v>
+        <v>48069.365</v>
       </c>
       <c r="U7" t="n">
-        <v>3197.9913</v>
+        <v>2424.0985</v>
       </c>
       <c r="V7" t="n">
-        <v>134.8209366666667</v>
+        <v>129.4333025</v>
       </c>
       <c r="W7" t="n">
-        <v>248.9355</v>
+        <v>246.512325</v>
       </c>
       <c r="X7" t="n">
-        <v>694.458</v>
+        <v>546.461275</v>
       </c>
       <c r="Y7" t="n">
-        <v>339.2614</v>
+        <v>334.0855</v>
       </c>
       <c r="Z7" t="n">
-        <v>372.8585666666666</v>
+        <v>374.9899</v>
       </c>
       <c r="AA7" t="n">
-        <v>460.4704333333333</v>
+        <v>457.335875</v>
       </c>
       <c r="AB7" t="n">
-        <v>930.0726333333333</v>
+        <v>772.66095</v>
       </c>
       <c r="AC7" t="n">
-        <v>392.9822333333333</v>
+        <v>407.3328</v>
       </c>
       <c r="AD7" t="n">
-        <v>519.8583666666667</v>
+        <v>482.19925</v>
       </c>
       <c r="AE7" t="n">
-        <v>384.1901333333333</v>
+        <v>368.99725</v>
       </c>
       <c r="AF7" t="n">
-        <v>1280727.866666667</v>
+        <v>978384.5975</v>
       </c>
       <c r="AG7" t="n">
         <v>10</v>
@@ -1209,94 +1209,94 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>566648917.5</v>
+        <v>453336053.026</v>
       </c>
       <c r="D8" t="n">
-        <v>3931208</v>
+        <v>2948422.5</v>
       </c>
       <c r="E8" t="n">
-        <v>1740.677033333333</v>
+        <v>1305.683291375</v>
       </c>
       <c r="F8" t="n">
-        <v>25.06631333333333</v>
+        <v>36.964905</v>
       </c>
       <c r="G8" t="n">
-        <v>35.70346666666666</v>
+        <v>36.06651</v>
       </c>
       <c r="H8" t="n">
-        <v>17.648793</v>
+        <v>22.28257725</v>
       </c>
       <c r="I8" t="n">
-        <v>78.16088999999999</v>
+        <v>68.5060225</v>
       </c>
       <c r="J8" t="n">
-        <v>46.69415666666666</v>
+        <v>46.488505</v>
       </c>
       <c r="K8" t="n">
-        <v>120.84693</v>
+        <v>92.5914765</v>
       </c>
       <c r="L8" t="n">
-        <v>1490.487666666667</v>
+        <v>1295.172225</v>
       </c>
       <c r="M8" t="n">
-        <v>185.46121</v>
+        <v>210.8499075</v>
       </c>
       <c r="N8" t="n">
-        <v>4731998.566666666</v>
+        <v>4056655.175</v>
       </c>
       <c r="O8" t="n">
-        <v>44503.55666666666</v>
+        <v>36222.8775</v>
       </c>
       <c r="P8" t="n">
-        <v>119.9076033333333</v>
+        <v>112.518715</v>
       </c>
       <c r="Q8" t="n">
-        <v>963.6284433333334</v>
+        <v>818.0974325</v>
       </c>
       <c r="R8" t="n">
-        <v>183.5077</v>
+        <v>192.10005</v>
       </c>
       <c r="S8" t="n">
-        <v>82.89663333333333</v>
+        <v>99.83132499999999</v>
       </c>
       <c r="T8" t="n">
-        <v>42674.46666666667</v>
+        <v>39030.4475</v>
       </c>
       <c r="U8" t="n">
-        <v>509.7605</v>
+        <v>405.3462375</v>
       </c>
       <c r="V8" t="n">
-        <v>106.4136033333333</v>
+        <v>107.0801025</v>
       </c>
       <c r="W8" t="n">
-        <v>247.1531333333333</v>
+        <v>245.1494</v>
       </c>
       <c r="X8" t="n">
-        <v>693.7094000000001</v>
+        <v>545.6558249999999</v>
       </c>
       <c r="Y8" t="n">
-        <v>338.3034</v>
+        <v>333.262375</v>
       </c>
       <c r="Z8" t="n">
-        <v>372.5463333333334</v>
+        <v>374.72955</v>
       </c>
       <c r="AA8" t="n">
-        <v>446.7449666666666</v>
+        <v>446.924425</v>
       </c>
       <c r="AB8" t="n">
-        <v>866.2063333333334</v>
+        <v>724.74225</v>
       </c>
       <c r="AC8" t="n">
-        <v>391.8569666666667</v>
+        <v>404.103775</v>
       </c>
       <c r="AD8" t="n">
-        <v>505.5689666666667</v>
+        <v>471.075025</v>
       </c>
       <c r="AE8" t="n">
-        <v>363.3962333333334</v>
+        <v>353.401825</v>
       </c>
       <c r="AF8" t="n">
-        <v>1268200.353333333</v>
+        <v>964935.3825000001</v>
       </c>
       <c r="AG8" t="n">
         <v>10</v>
@@ -1310,94 +1310,94 @@
         <v>40</v>
       </c>
       <c r="C9" t="n">
-        <v>554812792.5</v>
+        <v>443865361.308</v>
       </c>
       <c r="D9" t="n">
-        <v>3038682</v>
+        <v>2279027.75</v>
       </c>
       <c r="E9" t="n">
-        <v>1395.428366666667</v>
+        <v>1046.64832475</v>
       </c>
       <c r="F9" t="n">
-        <v>19.56523333333334</v>
+        <v>32.8255975</v>
       </c>
       <c r="G9" t="n">
-        <v>34.12332666666666</v>
+        <v>34.8062175</v>
       </c>
       <c r="H9" t="n">
-        <v>13.62654966666667</v>
+        <v>19.01653975</v>
       </c>
       <c r="I9" t="n">
-        <v>78.16088999999999</v>
+        <v>68.48983749999999</v>
       </c>
       <c r="J9" t="n">
-        <v>39.63919666666667</v>
+        <v>41.1929825</v>
       </c>
       <c r="K9" t="n">
-        <v>103.4865766666667</v>
+        <v>79.5680215</v>
       </c>
       <c r="L9" t="n">
-        <v>1408.494666666667</v>
+        <v>1233.553325</v>
       </c>
       <c r="M9" t="n">
-        <v>167.39461</v>
+        <v>196.9380575</v>
       </c>
       <c r="N9" t="n">
-        <v>3455834.233333333</v>
+        <v>3000729.925</v>
       </c>
       <c r="O9" t="n">
-        <v>44503.52666666666</v>
+        <v>36222.7925</v>
       </c>
       <c r="P9" t="n">
-        <v>109.1254333333333</v>
+        <v>97.9876075</v>
       </c>
       <c r="Q9" t="n">
-        <v>823.7237933333332</v>
+        <v>695.8818699999999</v>
       </c>
       <c r="R9" t="n">
-        <v>178.2539333333333</v>
+        <v>187.2208</v>
       </c>
       <c r="S9" t="n">
-        <v>82.89663333333333</v>
+        <v>79.69259</v>
       </c>
       <c r="T9" t="n">
-        <v>42605.45333333333</v>
+        <v>38978.6875</v>
       </c>
       <c r="U9" t="n">
-        <v>509.4332666666667</v>
+        <v>405.1008125</v>
       </c>
       <c r="V9" t="n">
-        <v>93.86183</v>
+        <v>97.1835975</v>
       </c>
       <c r="W9" t="n">
-        <v>247.1531333333333</v>
+        <v>245.13755</v>
       </c>
       <c r="X9" t="n">
-        <v>676.3579333333333</v>
+        <v>532.579025</v>
       </c>
       <c r="Y9" t="n">
-        <v>336.1137666666667</v>
+        <v>331.58485</v>
       </c>
       <c r="Z9" t="n">
-        <v>371.7933333333334</v>
+        <v>374.15165</v>
       </c>
       <c r="AA9" t="n">
-        <v>446.7449666666666</v>
+        <v>446.8985</v>
       </c>
       <c r="AB9" t="n">
-        <v>857.4763333333334</v>
+        <v>718.19475</v>
       </c>
       <c r="AC9" t="n">
-        <v>391.6720666666667</v>
+        <v>403.904975</v>
       </c>
       <c r="AD9" t="n">
-        <v>505.4050333333333</v>
+        <v>470.687725</v>
       </c>
       <c r="AE9" t="n">
-        <v>325.9426333333333</v>
+        <v>325.21165</v>
       </c>
       <c r="AF9" t="n">
-        <v>1160304.066666667</v>
+        <v>879534.46</v>
       </c>
       <c r="AG9" t="n">
         <v>10</v>
@@ -1411,94 +1411,94 @@
         <v>50</v>
       </c>
       <c r="C10" t="n">
-        <v>472250792.5</v>
+        <v>377807202.65</v>
       </c>
       <c r="D10" t="n">
-        <v>2767487</v>
+        <v>2075631.25</v>
       </c>
       <c r="E10" t="n">
-        <v>1261.433033333333</v>
+        <v>946.130560525</v>
       </c>
       <c r="F10" t="n">
-        <v>19.56523333333334</v>
+        <v>32.8140475</v>
       </c>
       <c r="G10" t="n">
-        <v>33.12309666666667</v>
+        <v>34.01003</v>
       </c>
       <c r="H10" t="n">
-        <v>12.46344966666667</v>
+        <v>18.11190225</v>
       </c>
       <c r="I10" t="n">
-        <v>73.29825666666666</v>
+        <v>64.82969750000001</v>
       </c>
       <c r="J10" t="n">
-        <v>38.57175666666667</v>
+        <v>40.388235</v>
       </c>
       <c r="K10" t="n">
-        <v>97.13361333333334</v>
+        <v>74.78090575</v>
       </c>
       <c r="L10" t="n">
-        <v>1316.139666666667</v>
+        <v>1164.162475</v>
       </c>
       <c r="M10" t="n">
-        <v>159.86191</v>
+        <v>190.9083575</v>
       </c>
       <c r="N10" t="n">
-        <v>3455834.233333333</v>
+        <v>2921967.175</v>
       </c>
       <c r="O10" t="n">
-        <v>44503.52666666666</v>
+        <v>36222.7925</v>
       </c>
       <c r="P10" t="n">
-        <v>91.27098666666666</v>
+        <v>84.5967725</v>
       </c>
       <c r="Q10" t="n">
-        <v>762.89386</v>
+        <v>649.6178199999999</v>
       </c>
       <c r="R10" t="n">
-        <v>174.3449</v>
+        <v>182.89045</v>
       </c>
       <c r="S10" t="n">
-        <v>71.81247</v>
+        <v>70.4391675</v>
       </c>
       <c r="T10" t="n">
-        <v>42444.84666666667</v>
+        <v>38858.2325</v>
       </c>
       <c r="U10" t="n">
-        <v>509.1351666666666</v>
+        <v>402.55052</v>
       </c>
       <c r="V10" t="n">
-        <v>92.17073000000001</v>
+        <v>95.31187250000001</v>
       </c>
       <c r="W10" t="n">
-        <v>244.6634</v>
+        <v>243.265475</v>
       </c>
       <c r="X10" t="n">
-        <v>673.0713333333333</v>
+        <v>530.0585</v>
       </c>
       <c r="Y10" t="n">
-        <v>335.1825666666667</v>
+        <v>330.839875</v>
       </c>
       <c r="Z10" t="n">
-        <v>371.7933333333334</v>
+        <v>374.13615</v>
       </c>
       <c r="AA10" t="n">
-        <v>445.7316</v>
+        <v>446.131825</v>
       </c>
       <c r="AB10" t="n">
-        <v>857.4763333333334</v>
+        <v>718.1513</v>
       </c>
       <c r="AC10" t="n">
-        <v>391.6594333333333</v>
+        <v>403.872875</v>
       </c>
       <c r="AD10" t="n">
-        <v>497.7466</v>
+        <v>464.8558</v>
       </c>
       <c r="AE10" t="n">
-        <v>319.0167</v>
+        <v>320.004825</v>
       </c>
       <c r="AF10" t="n">
-        <v>1160158.706666667</v>
+        <v>876226.6775</v>
       </c>
       <c r="AG10" t="n">
         <v>10</v>
@@ -1512,94 +1512,94 @@
         <v>60</v>
       </c>
       <c r="C11" t="n">
-        <v>444551665</v>
+        <v>355647723.092</v>
       </c>
       <c r="D11" t="n">
-        <v>724615.6666666666</v>
+        <v>543477.25</v>
       </c>
       <c r="E11" t="n">
-        <v>1261.433033333333</v>
+        <v>946.122527175</v>
       </c>
       <c r="F11" t="n">
-        <v>18.95103366666667</v>
+        <v>32.35203525</v>
       </c>
       <c r="G11" t="n">
-        <v>33.12309666666667</v>
+        <v>33.9231775</v>
       </c>
       <c r="H11" t="n">
-        <v>12.140534</v>
+        <v>17.824638</v>
       </c>
       <c r="I11" t="n">
-        <v>67.36800333333333</v>
+        <v>60.359655</v>
       </c>
       <c r="J11" t="n">
-        <v>37.95751333333333</v>
+        <v>39.92252</v>
       </c>
       <c r="K11" t="n">
-        <v>95.79225333333333</v>
+        <v>73.73945175</v>
       </c>
       <c r="L11" t="n">
-        <v>1010.460033333333</v>
+        <v>934.830875</v>
       </c>
       <c r="M11" t="n">
-        <v>159.8309633333333</v>
+        <v>190.2874975</v>
       </c>
       <c r="N11" t="n">
-        <v>3455834.233333333</v>
+        <v>2916684.175</v>
       </c>
       <c r="O11" t="n">
-        <v>44503.52666666666</v>
+        <v>36222.7925</v>
       </c>
       <c r="P11" t="n">
-        <v>91.27098666666666</v>
+        <v>84.5967725</v>
       </c>
       <c r="Q11" t="n">
-        <v>734.9086600000001</v>
+        <v>622.199445</v>
       </c>
       <c r="R11" t="n">
-        <v>170.9307333333333</v>
+        <v>168.460375</v>
       </c>
       <c r="S11" t="n">
-        <v>64.95195</v>
+        <v>61.62718750000001</v>
       </c>
       <c r="T11" t="n">
-        <v>38178.27</v>
+        <v>35658.27</v>
       </c>
       <c r="U11" t="n">
-        <v>400.8187333333333</v>
+        <v>320.272685</v>
       </c>
       <c r="V11" t="n">
-        <v>91.87766333333333</v>
+        <v>94.9240975</v>
       </c>
       <c r="W11" t="n">
-        <v>239.8679333333333</v>
+        <v>239.65185</v>
       </c>
       <c r="X11" t="n">
-        <v>673.0713333333333</v>
+        <v>530.04945</v>
       </c>
       <c r="Y11" t="n">
-        <v>334.5393</v>
+        <v>330.29745</v>
       </c>
       <c r="Z11" t="n">
-        <v>367.5732666666667</v>
+        <v>370.96755</v>
       </c>
       <c r="AA11" t="n">
-        <v>445.7316</v>
+        <v>446.131825</v>
       </c>
       <c r="AB11" t="n">
-        <v>826.5502333333334</v>
+        <v>694.9485999999999</v>
       </c>
       <c r="AC11" t="n">
-        <v>390.9794333333334</v>
+        <v>403.3627</v>
       </c>
       <c r="AD11" t="n">
-        <v>497.693</v>
+        <v>464.624125</v>
       </c>
       <c r="AE11" t="n">
-        <v>305.803</v>
+        <v>309.8504</v>
       </c>
       <c r="AF11" t="n">
-        <v>932912.7066666667</v>
+        <v>705427.6949999999</v>
       </c>
       <c r="AG11" t="n">
         <v>10</v>
@@ -1613,94 +1613,94 @@
         <v>70</v>
       </c>
       <c r="C12" t="n">
-        <v>444551665</v>
+        <v>355647723.092</v>
       </c>
       <c r="D12" t="n">
-        <v>724615.6666666666</v>
+        <v>543477.25</v>
       </c>
       <c r="E12" t="n">
-        <v>1227.7037</v>
+        <v>920.79071514</v>
       </c>
       <c r="F12" t="n">
-        <v>18.95103366666667</v>
+        <v>32.34827275</v>
       </c>
       <c r="G12" t="n">
-        <v>32.92989</v>
+        <v>33.70363</v>
       </c>
       <c r="H12" t="n">
-        <v>10.99044466666667</v>
+        <v>11.9818235</v>
       </c>
       <c r="I12" t="n">
-        <v>67.36800333333333</v>
+        <v>60.338645</v>
       </c>
       <c r="J12" t="n">
-        <v>37.95751333333333</v>
+        <v>39.92234</v>
       </c>
       <c r="K12" t="n">
-        <v>95.79225333333333</v>
+        <v>73.727318</v>
       </c>
       <c r="L12" t="n">
-        <v>1010.460033333333</v>
+        <v>934.797225</v>
       </c>
       <c r="M12" t="n">
-        <v>159.8309633333333</v>
+        <v>189.3899725</v>
       </c>
       <c r="N12" t="n">
-        <v>3455834.233333333</v>
+        <v>2897719.175</v>
       </c>
       <c r="O12" t="n">
-        <v>44503.52666666666</v>
+        <v>36222.7925</v>
       </c>
       <c r="P12" t="n">
-        <v>87.52087999999999</v>
+        <v>81.78419249999999</v>
       </c>
       <c r="Q12" t="n">
-        <v>734.09135</v>
+        <v>621.5833625</v>
       </c>
       <c r="R12" t="n">
-        <v>158.8442466666667</v>
+        <v>156.62011</v>
       </c>
       <c r="S12" t="n">
-        <v>64.95195</v>
+        <v>60.4250975</v>
       </c>
       <c r="T12" t="n">
-        <v>38178.27</v>
+        <v>35658.27</v>
       </c>
       <c r="U12" t="n">
-        <v>321.3539666666666</v>
+        <v>256.600755</v>
       </c>
       <c r="V12" t="n">
-        <v>91.87766333333333</v>
+        <v>94.9240975</v>
       </c>
       <c r="W12" t="n">
-        <v>239.7053333333333</v>
+        <v>239.5252</v>
       </c>
       <c r="X12" t="n">
-        <v>673.0713333333333</v>
+        <v>530.04855</v>
       </c>
       <c r="Y12" t="n">
-        <v>333.1672666666666</v>
+        <v>329.257175</v>
       </c>
       <c r="Z12" t="n">
-        <v>367.5732666666667</v>
+        <v>361.5284</v>
       </c>
       <c r="AA12" t="n">
-        <v>441.1143</v>
+        <v>442.664225</v>
       </c>
       <c r="AB12" t="n">
-        <v>826.5502333333334</v>
+        <v>694.94675</v>
       </c>
       <c r="AC12" t="n">
-        <v>390.9794333333334</v>
+        <v>403.361925</v>
       </c>
       <c r="AD12" t="n">
-        <v>497.6824</v>
+        <v>464.384625</v>
       </c>
       <c r="AE12" t="n">
-        <v>304.4019333333333</v>
+        <v>308.787025</v>
       </c>
       <c r="AF12" t="n">
-        <v>924238.59</v>
+        <v>698837.5125</v>
       </c>
       <c r="AG12" t="n">
         <v>10</v>
@@ -1714,94 +1714,94 @@
         <v>80</v>
       </c>
       <c r="C13" t="n">
-        <v>444551665</v>
+        <v>355647671.6</v>
       </c>
       <c r="D13" t="n">
-        <v>722675.6666666666</v>
+        <v>542022</v>
       </c>
       <c r="E13" t="n">
-        <v>1227.7037</v>
+        <v>920.7842566575</v>
       </c>
       <c r="F13" t="n">
-        <v>18.95103366666667</v>
+        <v>32.34200525</v>
       </c>
       <c r="G13" t="n">
-        <v>32.92989</v>
+        <v>33.5700575</v>
       </c>
       <c r="H13" t="n">
-        <v>10.44419133333333</v>
+        <v>11.346316</v>
       </c>
       <c r="I13" t="n">
-        <v>67.36800333333333</v>
+        <v>60.33798</v>
       </c>
       <c r="J13" t="n">
-        <v>36.70078</v>
+        <v>38.9792775</v>
       </c>
       <c r="K13" t="n">
-        <v>95.79225333333333</v>
+        <v>73.70186074999999</v>
       </c>
       <c r="L13" t="n">
-        <v>1010.460033333333</v>
+        <v>934.7849</v>
       </c>
       <c r="M13" t="n">
-        <v>150.4825533333333</v>
+        <v>129.4982725</v>
       </c>
       <c r="N13" t="n">
-        <v>3380718.233333333</v>
+        <v>2811244.925</v>
       </c>
       <c r="O13" t="n">
-        <v>44502.68333333333</v>
+        <v>36222.16</v>
       </c>
       <c r="P13" t="n">
-        <v>70.00276333333333</v>
+        <v>68.64560499999999</v>
       </c>
       <c r="Q13" t="n">
-        <v>678.1455533333333</v>
+        <v>579.624015</v>
       </c>
       <c r="R13" t="n">
-        <v>158.8442466666667</v>
+        <v>156.06246</v>
       </c>
       <c r="S13" t="n">
-        <v>56.03356</v>
+        <v>53.2920525</v>
       </c>
       <c r="T13" t="n">
-        <v>37691.09666666667</v>
+        <v>35292.89</v>
       </c>
       <c r="U13" t="n">
-        <v>321.3539666666666</v>
+        <v>256.321225</v>
       </c>
       <c r="V13" t="n">
-        <v>86.70908000000001</v>
+        <v>91.04766000000001</v>
       </c>
       <c r="W13" t="n">
-        <v>237.3008666666667</v>
+        <v>237.717125</v>
       </c>
       <c r="X13" t="n">
-        <v>660.4253333333332</v>
+        <v>520.5608</v>
       </c>
       <c r="Y13" t="n">
-        <v>333.1672666666666</v>
+        <v>329.22485</v>
       </c>
       <c r="Z13" t="n">
-        <v>367.5732666666667</v>
+        <v>360.97075</v>
       </c>
       <c r="AA13" t="n">
-        <v>441.1143</v>
+        <v>442.663975</v>
       </c>
       <c r="AB13" t="n">
-        <v>823.8107333333334</v>
+        <v>692.88165</v>
       </c>
       <c r="AC13" t="n">
-        <v>390.9794333333334</v>
+        <v>403.3457</v>
       </c>
       <c r="AD13" t="n">
-        <v>497.5073666666667</v>
+        <v>463.699875</v>
       </c>
       <c r="AE13" t="n">
-        <v>297.9873</v>
+        <v>303.886575</v>
       </c>
       <c r="AF13" t="n">
-        <v>924238.59</v>
+        <v>698837.0475</v>
       </c>
       <c r="AG13" t="n">
         <v>10</v>
@@ -1815,94 +1815,94 @@
         <v>90</v>
       </c>
       <c r="C14" t="n">
-        <v>297007465</v>
+        <v>237610583.738</v>
       </c>
       <c r="D14" t="n">
-        <v>699082</v>
+        <v>524326</v>
       </c>
       <c r="E14" t="n">
-        <v>1227.7037</v>
+        <v>920.782640885</v>
       </c>
       <c r="F14" t="n">
-        <v>18.87817366666667</v>
+        <v>32.28477775</v>
       </c>
       <c r="G14" t="n">
-        <v>32.92989</v>
+        <v>33.49910250000001</v>
       </c>
       <c r="H14" t="n">
-        <v>10.44419133333333</v>
+        <v>11.338756</v>
       </c>
       <c r="I14" t="n">
-        <v>67.36800333333333</v>
+        <v>60.334615</v>
       </c>
       <c r="J14" t="n">
-        <v>36.70078</v>
+        <v>38.97801</v>
       </c>
       <c r="K14" t="n">
-        <v>89.08792999999999</v>
+        <v>68.65913499999999</v>
       </c>
       <c r="L14" t="n">
-        <v>1010.460033333333</v>
+        <v>934.7708749999999</v>
       </c>
       <c r="M14" t="n">
-        <v>147.82002</v>
+        <v>122.783685</v>
       </c>
       <c r="N14" t="n">
-        <v>3380718.233333333</v>
+        <v>2798039.925</v>
       </c>
       <c r="O14" t="n">
-        <v>43462.23666666666</v>
+        <v>35441.825</v>
       </c>
       <c r="P14" t="n">
-        <v>70.00276333333333</v>
+        <v>68.59913</v>
       </c>
       <c r="Q14" t="n">
-        <v>591.2696533333334</v>
+        <v>512.865465</v>
       </c>
       <c r="R14" t="n">
-        <v>158.8442466666667</v>
+        <v>155.92346</v>
       </c>
       <c r="S14" t="n">
-        <v>51.74518666666668</v>
+        <v>49.9745575</v>
       </c>
       <c r="T14" t="n">
-        <v>34105.43333333333</v>
+        <v>32603.6425</v>
       </c>
       <c r="U14" t="n">
-        <v>302.2129666666667</v>
+        <v>241.965475</v>
       </c>
       <c r="V14" t="n">
-        <v>51.29524333333333</v>
+        <v>64.48728249999999</v>
       </c>
       <c r="W14" t="n">
-        <v>236.3963666666667</v>
+        <v>237.034275</v>
       </c>
       <c r="X14" t="n">
-        <v>660.4253333333332</v>
+        <v>520.5454999999999</v>
       </c>
       <c r="Y14" t="n">
-        <v>333.1672666666666</v>
+        <v>329.20565</v>
       </c>
       <c r="Z14" t="n">
-        <v>366.5188333333334</v>
+        <v>360.1277</v>
       </c>
       <c r="AA14" t="n">
-        <v>440.6991666666666</v>
+        <v>442.35025</v>
       </c>
       <c r="AB14" t="n">
-        <v>820.9157333333333</v>
+        <v>690.7056</v>
       </c>
       <c r="AC14" t="n">
-        <v>390.7537333333333</v>
+        <v>403.169825</v>
       </c>
       <c r="AD14" t="n">
-        <v>497.4596999999999</v>
+        <v>452.637175</v>
       </c>
       <c r="AE14" t="n">
-        <v>297.9873</v>
+        <v>303.88625</v>
       </c>
       <c r="AF14" t="n">
-        <v>924238.59</v>
+        <v>698819.8625</v>
       </c>
       <c r="AG14" t="n">
         <v>10</v>
@@ -1916,94 +1916,94 @@
         <v>100</v>
       </c>
       <c r="C15" t="n">
-        <v>297007465</v>
+        <v>237608666.73</v>
       </c>
       <c r="D15" t="n">
-        <v>698477.6666666666</v>
+        <v>523872.25</v>
       </c>
       <c r="E15" t="n">
-        <v>1160.7656</v>
+        <v>870.57620893275</v>
       </c>
       <c r="F15" t="n">
-        <v>13.29269033333333</v>
+        <v>28.08489025</v>
       </c>
       <c r="G15" t="n">
-        <v>27.36746333333333</v>
+        <v>29.3117475</v>
       </c>
       <c r="H15" t="n">
-        <v>10.44419133333333</v>
+        <v>11.338446</v>
       </c>
       <c r="I15" t="n">
-        <v>67.36800333333333</v>
+        <v>60.32916</v>
       </c>
       <c r="J15" t="n">
-        <v>36.70078</v>
+        <v>38.975895</v>
       </c>
       <c r="K15" t="n">
-        <v>89.08792999999999</v>
+        <v>68.6494355</v>
       </c>
       <c r="L15" t="n">
-        <v>1010.460033333333</v>
+        <v>934.767325</v>
       </c>
       <c r="M15" t="n">
-        <v>147.82002</v>
+        <v>122.693655</v>
       </c>
       <c r="N15" t="n">
-        <v>3377578.166666667</v>
+        <v>2794531.875</v>
       </c>
       <c r="O15" t="n">
-        <v>43462.23666666666</v>
+        <v>35441.825</v>
       </c>
       <c r="P15" t="n">
-        <v>70.00276333333333</v>
+        <v>68.5678875</v>
       </c>
       <c r="Q15" t="n">
-        <v>434.0759866666667</v>
+        <v>394.667015</v>
       </c>
       <c r="R15" t="n">
-        <v>158.8442466666667</v>
+        <v>155.599685</v>
       </c>
       <c r="S15" t="n">
-        <v>51.42884666666667</v>
+        <v>49.7141</v>
       </c>
       <c r="T15" t="n">
-        <v>32653.90333333333</v>
+        <v>31514.995</v>
       </c>
       <c r="U15" t="n">
-        <v>297.9023</v>
+        <v>238.732475</v>
       </c>
       <c r="V15" t="n">
-        <v>51.29524333333333</v>
+        <v>64.4072575</v>
       </c>
       <c r="W15" t="n">
-        <v>236.3963666666667</v>
+        <v>237.0319</v>
       </c>
       <c r="X15" t="n">
-        <v>660.4253333333332</v>
+        <v>520.543425</v>
       </c>
       <c r="Y15" t="n">
-        <v>331.9504666666667</v>
+        <v>328.28975</v>
       </c>
       <c r="Z15" t="n">
-        <v>362.6881333333333</v>
+        <v>357.24205</v>
       </c>
       <c r="AA15" t="n">
-        <v>440.0640333333333</v>
+        <v>441.8738</v>
       </c>
       <c r="AB15" t="n">
-        <v>820.9157333333333</v>
+        <v>690.704375</v>
       </c>
       <c r="AC15" t="n">
-        <v>390.6434333333333</v>
+        <v>403.076625</v>
       </c>
       <c r="AD15" t="n">
-        <v>497.4596999999999</v>
+        <v>448.54445</v>
       </c>
       <c r="AE15" t="n">
-        <v>297.9873</v>
+        <v>303.40885</v>
       </c>
       <c r="AF15" t="n">
-        <v>699718.59</v>
+        <v>530403.14</v>
       </c>
       <c r="AG15" t="n">
         <v>10</v>

</xml_diff>

<commit_message>
v4&v5 : chaotic operators
</commit_message>
<xml_diff>
--- a/cec2017real-master/code/results_ARO/results_cec2017_10.xlsx
+++ b/cec2017real-master/code/results_ARO/results_cec2017_10.xlsx
@@ -603,94 +603,94 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>826528306</v>
+        <v>514057010.7142857</v>
       </c>
       <c r="D2" t="n">
-        <v>2436064906.25</v>
+        <v>7.335251538472529e+20</v>
       </c>
       <c r="E2" t="n">
-        <v>20770.0275</v>
+        <v>18502.75723076923</v>
       </c>
       <c r="F2" t="n">
-        <v>80.33364</v>
+        <v>105.2249369230769</v>
       </c>
       <c r="G2" t="n">
-        <v>60.7313275</v>
+        <v>63.52591692307692</v>
       </c>
       <c r="H2" t="n">
-        <v>46.733985</v>
+        <v>42.08338769230769</v>
       </c>
       <c r="I2" t="n">
-        <v>115.214485</v>
+        <v>106.49537</v>
       </c>
       <c r="J2" t="n">
-        <v>71.5203475</v>
+        <v>70.08794916666666</v>
       </c>
       <c r="K2" t="n">
-        <v>291.243275</v>
+        <v>632.4441416666667</v>
       </c>
       <c r="L2" t="n">
-        <v>1660.363225</v>
+        <v>1618.996908333333</v>
       </c>
       <c r="M2" t="n">
-        <v>413.169575</v>
+        <v>2573.3987</v>
       </c>
       <c r="N2" t="n">
-        <v>30188255</v>
+        <v>16672944.16666667</v>
       </c>
       <c r="O2" t="n">
-        <v>334101.8875</v>
+        <v>208320.7727272727</v>
       </c>
       <c r="P2" t="n">
-        <v>6667.700750000001</v>
+        <v>10075.695</v>
       </c>
       <c r="Q2" t="n">
-        <v>57840.08275</v>
+        <v>37229.72763636363</v>
       </c>
       <c r="R2" t="n">
-        <v>373.939675</v>
+        <v>419.7384545454545</v>
       </c>
       <c r="S2" t="n">
-        <v>187.9202</v>
+        <v>201.3324909090909</v>
       </c>
       <c r="T2" t="n">
-        <v>778568.845</v>
+        <v>750088.24</v>
       </c>
       <c r="U2" t="n">
-        <v>29524.58975</v>
+        <v>155105.4617272727</v>
       </c>
       <c r="V2" t="n">
-        <v>338.500175</v>
+        <v>245.2891545454545</v>
       </c>
       <c r="W2" t="n">
-        <v>264.00015</v>
+        <v>267.8236272727273</v>
       </c>
       <c r="X2" t="n">
-        <v>690.643375</v>
+        <v>549.1421600000001</v>
       </c>
       <c r="Y2" t="n">
-        <v>375.728575</v>
+        <v>370.65069</v>
       </c>
       <c r="Z2" t="n">
-        <v>396.547875</v>
+        <v>404.30287</v>
       </c>
       <c r="AA2" t="n">
-        <v>479.080325</v>
+        <v>478.8247666666666</v>
       </c>
       <c r="AB2" t="n">
-        <v>962.647425</v>
+        <v>1009.562222222222</v>
       </c>
       <c r="AC2" t="n">
-        <v>421.68175</v>
+        <v>421.2585444444445</v>
       </c>
       <c r="AD2" t="n">
-        <v>527.0715250000001</v>
+        <v>685.8185555555556</v>
       </c>
       <c r="AE2" t="n">
-        <v>503.4609</v>
+        <v>475.0039444444444</v>
       </c>
       <c r="AF2" t="n">
-        <v>7249508</v>
+        <v>4372969.977777777</v>
       </c>
       <c r="AG2" t="n">
         <v>10</v>
@@ -704,94 +704,94 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>757792392.6</v>
+        <v>347358945.2142857</v>
       </c>
       <c r="D3" t="n">
-        <v>720558647.75</v>
+        <v>7.335251538464206e+20</v>
       </c>
       <c r="E3" t="n">
-        <v>10756.402</v>
+        <v>9550.039692307693</v>
       </c>
       <c r="F3" t="n">
-        <v>64.9858825</v>
+        <v>54.20821676923077</v>
       </c>
       <c r="G3" t="n">
-        <v>56.8046525</v>
+        <v>57.69587692307692</v>
       </c>
       <c r="H3" t="n">
-        <v>28.7369475</v>
+        <v>31.77571923076923</v>
       </c>
       <c r="I3" t="n">
-        <v>104.20841</v>
+        <v>93.47149</v>
       </c>
       <c r="J3" t="n">
-        <v>63.0274475</v>
+        <v>53.71772666666666</v>
       </c>
       <c r="K3" t="n">
-        <v>168.71062</v>
+        <v>480.1448983333333</v>
       </c>
       <c r="L3" t="n">
-        <v>1616.336225</v>
+        <v>1474.88585</v>
       </c>
       <c r="M3" t="n">
-        <v>274.047025</v>
+        <v>1331.611190833333</v>
       </c>
       <c r="N3" t="n">
-        <v>21628805.75</v>
+        <v>10869403.91666667</v>
       </c>
       <c r="O3" t="n">
-        <v>112920.165</v>
+        <v>68797.69372727274</v>
       </c>
       <c r="P3" t="n">
-        <v>6437.650025000001</v>
+        <v>8322.803736363638</v>
       </c>
       <c r="Q3" t="n">
-        <v>30801.7995</v>
+        <v>24407.11118181818</v>
       </c>
       <c r="R3" t="n">
-        <v>252.9839</v>
+        <v>330.1615818181818</v>
       </c>
       <c r="S3" t="n">
-        <v>161.324525</v>
+        <v>186.5198445454545</v>
       </c>
       <c r="T3" t="n">
-        <v>316436.29</v>
+        <v>158555.4772727273</v>
       </c>
       <c r="U3" t="n">
-        <v>16039.66025</v>
+        <v>137606.8191818182</v>
       </c>
       <c r="V3" t="n">
-        <v>252.97155</v>
+        <v>201.6637390909091</v>
       </c>
       <c r="W3" t="n">
-        <v>257.774825</v>
+        <v>262.3417363636364</v>
       </c>
       <c r="X3" t="n">
-        <v>648.4328250000001</v>
+        <v>500.38508</v>
       </c>
       <c r="Y3" t="n">
-        <v>351.0404</v>
+        <v>350.17759</v>
       </c>
       <c r="Z3" t="n">
-        <v>391.21795</v>
+        <v>400.48717</v>
       </c>
       <c r="AA3" t="n">
-        <v>472.19895</v>
+        <v>464.7235444444445</v>
       </c>
       <c r="AB3" t="n">
-        <v>847.669525</v>
+        <v>913.686111111111</v>
       </c>
       <c r="AC3" t="n">
-        <v>419.954475</v>
+        <v>414.5715666666667</v>
       </c>
       <c r="AD3" t="n">
-        <v>519.567175</v>
+        <v>674.1730777777778</v>
       </c>
       <c r="AE3" t="n">
-        <v>464.25405</v>
+        <v>452.6315111111111</v>
       </c>
       <c r="AF3" t="n">
-        <v>3312836.25</v>
+        <v>2152950.633333333</v>
       </c>
       <c r="AG3" t="n">
         <v>10</v>
@@ -805,94 +805,94 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>740643774.6</v>
+        <v>316515747.3571429</v>
       </c>
       <c r="D4" t="n">
-        <v>44948152.75</v>
+        <v>7.335251538461794e+20</v>
       </c>
       <c r="E4" t="n">
-        <v>5890.3485</v>
+        <v>6146.920692307692</v>
       </c>
       <c r="F4" t="n">
-        <v>59.387545</v>
+        <v>42.12647746153846</v>
       </c>
       <c r="G4" t="n">
-        <v>56.17666</v>
+        <v>53.87009923076923</v>
       </c>
       <c r="H4" t="n">
-        <v>25.88164</v>
+        <v>26.67367692307692</v>
       </c>
       <c r="I4" t="n">
-        <v>100.9850275</v>
+        <v>86.96486083333333</v>
       </c>
       <c r="J4" t="n">
-        <v>55.99485</v>
+        <v>48.33890583333334</v>
       </c>
       <c r="K4" t="n">
-        <v>166.1480925</v>
+        <v>448.4222475</v>
       </c>
       <c r="L4" t="n">
-        <v>1597.909325</v>
+        <v>1412.73135</v>
       </c>
       <c r="M4" t="n">
-        <v>248.195495</v>
+        <v>938.0563908333334</v>
       </c>
       <c r="N4" t="n">
-        <v>18751916.75</v>
+        <v>9399959.141666668</v>
       </c>
       <c r="O4" t="n">
-        <v>112897.04</v>
+        <v>55535.03018181818</v>
       </c>
       <c r="P4" t="n">
-        <v>5046.208575</v>
+        <v>6305.510436363636</v>
       </c>
       <c r="Q4" t="n">
-        <v>22065.7595</v>
+        <v>15933.54009090909</v>
       </c>
       <c r="R4" t="n">
-        <v>218.619525</v>
+        <v>282.9929454545455</v>
       </c>
       <c r="S4" t="n">
-        <v>160.1275</v>
+        <v>182.8646945454545</v>
       </c>
       <c r="T4" t="n">
-        <v>145911.07</v>
+        <v>83336.73818181817</v>
       </c>
       <c r="U4" t="n">
-        <v>14021.28</v>
+        <v>121196.9237272727</v>
       </c>
       <c r="V4" t="n">
-        <v>187.01936</v>
+        <v>173.3110072727273</v>
       </c>
       <c r="W4" t="n">
-        <v>254.039075</v>
+        <v>241.3578636363636</v>
       </c>
       <c r="X4" t="n">
-        <v>648.2886000000001</v>
+        <v>493.00418</v>
       </c>
       <c r="Y4" t="n">
-        <v>347.241275</v>
+        <v>346.74783</v>
       </c>
       <c r="Z4" t="n">
-        <v>385.548375</v>
+        <v>389.6665777777778</v>
       </c>
       <c r="AA4" t="n">
-        <v>471.596925</v>
+        <v>463.2507777777777</v>
       </c>
       <c r="AB4" t="n">
-        <v>812.737</v>
+        <v>876.5403666666666</v>
       </c>
       <c r="AC4" t="n">
-        <v>419.33375</v>
+        <v>413.3439222222222</v>
       </c>
       <c r="AD4" t="n">
-        <v>514.801325</v>
+        <v>652.4334666666667</v>
       </c>
       <c r="AE4" t="n">
-        <v>461.27145</v>
+        <v>449.6809444444444</v>
       </c>
       <c r="AF4" t="n">
-        <v>3155519</v>
+        <v>1939309.988888889</v>
       </c>
       <c r="AG4" t="n">
         <v>10</v>
@@ -906,94 +906,94 @@
         <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>738063492.6</v>
+        <v>278877422.5</v>
       </c>
       <c r="D5" t="n">
-        <v>32502751</v>
+        <v>7.335251538461655e+20</v>
       </c>
       <c r="E5" t="n">
-        <v>3767.74895</v>
+        <v>4228.362061538462</v>
       </c>
       <c r="F5" t="n">
-        <v>56.1555025</v>
+        <v>35.66981323076923</v>
       </c>
       <c r="G5" t="n">
-        <v>51.7026425</v>
+        <v>48.82960153846154</v>
       </c>
       <c r="H5" t="n">
-        <v>23.6674925</v>
+        <v>24.66060638461538</v>
       </c>
       <c r="I5" t="n">
-        <v>92.75526499999999</v>
+        <v>81.21223833333333</v>
       </c>
       <c r="J5" t="n">
-        <v>54.3618775</v>
+        <v>45.76101</v>
       </c>
       <c r="K5" t="n">
-        <v>159.9836625</v>
+        <v>263.0703541666667</v>
       </c>
       <c r="L5" t="n">
-        <v>1447.1329</v>
+        <v>1304.422391666667</v>
       </c>
       <c r="M5" t="n">
-        <v>245.3338375</v>
+        <v>536.3988566666667</v>
       </c>
       <c r="N5" t="n">
-        <v>12024384</v>
+        <v>6768836.325</v>
       </c>
       <c r="O5" t="n">
-        <v>96622.72749999999</v>
+        <v>38740.74963636364</v>
       </c>
       <c r="P5" t="n">
-        <v>3178.52515</v>
+        <v>3304.478136363636</v>
       </c>
       <c r="Q5" t="n">
-        <v>10295.763</v>
+        <v>8569.526118181819</v>
       </c>
       <c r="R5" t="n">
-        <v>205.452325</v>
+        <v>252.1971545454546</v>
       </c>
       <c r="S5" t="n">
-        <v>149.6699</v>
+        <v>173.9616318181818</v>
       </c>
       <c r="T5" t="n">
-        <v>137386.1625</v>
+        <v>67662.87645454545</v>
       </c>
       <c r="U5" t="n">
-        <v>13900.053</v>
+        <v>112353.4262727273</v>
       </c>
       <c r="V5" t="n">
-        <v>165.75138</v>
+        <v>157.4311118181818</v>
       </c>
       <c r="W5" t="n">
-        <v>251.1193</v>
+        <v>223.9785090909091</v>
       </c>
       <c r="X5" t="n">
-        <v>611.22965</v>
+        <v>456.85152</v>
       </c>
       <c r="Y5" t="n">
-        <v>341.085775</v>
+        <v>342.46827</v>
       </c>
       <c r="Z5" t="n">
-        <v>377.893475</v>
+        <v>383.5603777777778</v>
       </c>
       <c r="AA5" t="n">
-        <v>467.09275</v>
+        <v>459.8778666666667</v>
       </c>
       <c r="AB5" t="n">
-        <v>787.524775</v>
+        <v>759.0975888888889</v>
       </c>
       <c r="AC5" t="n">
-        <v>416.081525</v>
+        <v>410.6204666666667</v>
       </c>
       <c r="AD5" t="n">
-        <v>513.7828499999999</v>
+        <v>627.1615111111111</v>
       </c>
       <c r="AE5" t="n">
-        <v>391.27645</v>
+        <v>393.1554</v>
       </c>
       <c r="AF5" t="n">
-        <v>2977958.5</v>
+        <v>1806153.866666667</v>
       </c>
       <c r="AG5" t="n">
         <v>10</v>
@@ -1007,94 +1007,94 @@
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>609518145.96</v>
+        <v>222311561.2</v>
       </c>
       <c r="D6" t="n">
-        <v>12349515.25</v>
+        <v>7.335251538461579e+20</v>
       </c>
       <c r="E6" t="n">
-        <v>2744.3232725</v>
+        <v>2727.039645384616</v>
       </c>
       <c r="F6" t="n">
-        <v>42.3586925</v>
+        <v>24.17667869230769</v>
       </c>
       <c r="G6" t="n">
-        <v>45.3392275</v>
+        <v>44.50936153846154</v>
       </c>
       <c r="H6" t="n">
-        <v>23.4605825</v>
+        <v>23.33378784615385</v>
       </c>
       <c r="I6" t="n">
-        <v>84.65531</v>
+        <v>71.233935</v>
       </c>
       <c r="J6" t="n">
-        <v>52.473335</v>
+        <v>41.54786</v>
       </c>
       <c r="K6" t="n">
-        <v>113.48621375</v>
+        <v>142.85824625</v>
       </c>
       <c r="L6" t="n">
-        <v>1417.09785</v>
+        <v>1230.066475</v>
       </c>
       <c r="M6" t="n">
-        <v>238.052645</v>
+        <v>295.1185991666667</v>
       </c>
       <c r="N6" t="n">
-        <v>9597429.75</v>
+        <v>5585814.566666666</v>
       </c>
       <c r="O6" t="n">
-        <v>94134.48</v>
+        <v>37273.86463636364</v>
       </c>
       <c r="P6" t="n">
-        <v>260.0064</v>
+        <v>1412.910090909091</v>
       </c>
       <c r="Q6" t="n">
-        <v>3584.96825</v>
+        <v>5100.098845454545</v>
       </c>
       <c r="R6" t="n">
-        <v>200.59105</v>
+        <v>244.2448727272727</v>
       </c>
       <c r="S6" t="n">
-        <v>137.384225</v>
+        <v>168.3506654545455</v>
       </c>
       <c r="T6" t="n">
-        <v>129563.91</v>
+        <v>60114.519</v>
       </c>
       <c r="U6" t="n">
-        <v>4161.1053</v>
+        <v>99873.57246363637</v>
       </c>
       <c r="V6" t="n">
-        <v>152.26303</v>
+        <v>148.9602854545454</v>
       </c>
       <c r="W6" t="n">
-        <v>250.0349</v>
+        <v>206.3831090909091</v>
       </c>
       <c r="X6" t="n">
-        <v>604.6635</v>
+        <v>447.45756</v>
       </c>
       <c r="Y6" t="n">
-        <v>338.322575</v>
+        <v>340.75902</v>
       </c>
       <c r="Z6" t="n">
-        <v>377.49375</v>
+        <v>379.2938777777778</v>
       </c>
       <c r="AA6" t="n">
-        <v>458.143875</v>
+        <v>453.5647111111111</v>
       </c>
       <c r="AB6" t="n">
-        <v>783.2268</v>
+        <v>726.8013555555556</v>
       </c>
       <c r="AC6" t="n">
-        <v>414.596</v>
+        <v>408.8094333333333</v>
       </c>
       <c r="AD6" t="n">
-        <v>510.93615</v>
+        <v>492.3025666666667</v>
       </c>
       <c r="AE6" t="n">
-        <v>378.43775</v>
+        <v>381.2911</v>
       </c>
       <c r="AF6" t="n">
-        <v>2050010.3</v>
+        <v>1325395.433333333</v>
       </c>
       <c r="AG6" t="n">
         <v>10</v>
@@ -1108,94 +1108,94 @@
         <v>20</v>
       </c>
       <c r="C7" t="n">
-        <v>482485646.1</v>
+        <v>174348272.3214286</v>
       </c>
       <c r="D7" t="n">
-        <v>9625953</v>
+        <v>18022107.53846154</v>
       </c>
       <c r="E7" t="n">
-        <v>1451.4752995</v>
+        <v>1393.327369076923</v>
       </c>
       <c r="F7" t="n">
-        <v>36.97904</v>
+        <v>18.54309869230769</v>
       </c>
       <c r="G7" t="n">
-        <v>40.2909875</v>
+        <v>41.26291846153846</v>
       </c>
       <c r="H7" t="n">
-        <v>22.71446275</v>
+        <v>22.45032569230769</v>
       </c>
       <c r="I7" t="n">
-        <v>79.7488225</v>
+        <v>64.75365833333333</v>
       </c>
       <c r="J7" t="n">
-        <v>47.2369225</v>
+        <v>37.08339083333333</v>
       </c>
       <c r="K7" t="n">
-        <v>109.21415525</v>
+        <v>117.83650275</v>
       </c>
       <c r="L7" t="n">
-        <v>1323.46</v>
+        <v>1181.790433333333</v>
       </c>
       <c r="M7" t="n">
-        <v>212.04367</v>
+        <v>151.8204458333333</v>
       </c>
       <c r="N7" t="n">
-        <v>4086986.325</v>
+        <v>3493977.725</v>
       </c>
       <c r="O7" t="n">
-        <v>36224.3025</v>
+        <v>15723.31806363636</v>
       </c>
       <c r="P7" t="n">
-        <v>195.42065</v>
+        <v>703.6860427272727</v>
       </c>
       <c r="Q7" t="n">
-        <v>926.93751</v>
+        <v>3167.872567272727</v>
       </c>
       <c r="R7" t="n">
-        <v>195.804625</v>
+        <v>198.1269354545455</v>
       </c>
       <c r="S7" t="n">
-        <v>99.87965</v>
+        <v>142.3520354545454</v>
       </c>
       <c r="T7" t="n">
-        <v>48069.365</v>
+        <v>29108.53609090909</v>
       </c>
       <c r="U7" t="n">
-        <v>2424.0985</v>
+        <v>65222.04230909091</v>
       </c>
       <c r="V7" t="n">
-        <v>129.4333025</v>
+        <v>133.4750954545455</v>
       </c>
       <c r="W7" t="n">
-        <v>246.512325</v>
+        <v>202.2521909090909</v>
       </c>
       <c r="X7" t="n">
-        <v>546.461275</v>
+        <v>422.69424</v>
       </c>
       <c r="Y7" t="n">
-        <v>334.0855</v>
+        <v>335.21546</v>
       </c>
       <c r="Z7" t="n">
-        <v>374.9899</v>
+        <v>374.8695333333333</v>
       </c>
       <c r="AA7" t="n">
-        <v>457.335875</v>
+        <v>449.4067</v>
       </c>
       <c r="AB7" t="n">
-        <v>772.66095</v>
+        <v>591.719788888889</v>
       </c>
       <c r="AC7" t="n">
-        <v>407.3328</v>
+        <v>404.4055666666666</v>
       </c>
       <c r="AD7" t="n">
-        <v>482.19925</v>
+        <v>452.4159888888889</v>
       </c>
       <c r="AE7" t="n">
-        <v>368.99725</v>
+        <v>366.5682222222222</v>
       </c>
       <c r="AF7" t="n">
-        <v>978384.5975</v>
+        <v>648569.9133333333</v>
       </c>
       <c r="AG7" t="n">
         <v>10</v>
@@ -1209,94 +1209,94 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>453336053.026</v>
+        <v>163282598.5807143</v>
       </c>
       <c r="D8" t="n">
-        <v>2948422.5</v>
+        <v>3733155.153846154</v>
       </c>
       <c r="E8" t="n">
-        <v>1305.683291375</v>
+        <v>885.5438827307693</v>
       </c>
       <c r="F8" t="n">
-        <v>36.964905</v>
+        <v>15.90442961538462</v>
       </c>
       <c r="G8" t="n">
-        <v>36.06651</v>
+        <v>39.32365692307692</v>
       </c>
       <c r="H8" t="n">
-        <v>22.28257725</v>
+        <v>22.05790707692308</v>
       </c>
       <c r="I8" t="n">
-        <v>68.5060225</v>
+        <v>57.891435</v>
       </c>
       <c r="J8" t="n">
-        <v>46.488505</v>
+        <v>35.6002925</v>
       </c>
       <c r="K8" t="n">
-        <v>92.5914765</v>
+        <v>101.5747104166667</v>
       </c>
       <c r="L8" t="n">
-        <v>1295.172225</v>
+        <v>1132.52335</v>
       </c>
       <c r="M8" t="n">
-        <v>210.8499075</v>
+        <v>131.7064233333333</v>
       </c>
       <c r="N8" t="n">
-        <v>4056655.175</v>
+        <v>3466713.272727273</v>
       </c>
       <c r="O8" t="n">
-        <v>36222.8775</v>
+        <v>15640.25542727273</v>
       </c>
       <c r="P8" t="n">
-        <v>112.518715</v>
+        <v>426.7442918181818</v>
       </c>
       <c r="Q8" t="n">
-        <v>818.0974325</v>
+        <v>2445.140693636364</v>
       </c>
       <c r="R8" t="n">
-        <v>192.10005</v>
+        <v>194.3661084545454</v>
       </c>
       <c r="S8" t="n">
-        <v>99.83132499999999</v>
+        <v>137.8351272727273</v>
       </c>
       <c r="T8" t="n">
-        <v>39030.4475</v>
+        <v>24948.95809090909</v>
       </c>
       <c r="U8" t="n">
-        <v>405.3462375</v>
+        <v>59679.29996818181</v>
       </c>
       <c r="V8" t="n">
-        <v>107.0801025</v>
+        <v>123.8666854545454</v>
       </c>
       <c r="W8" t="n">
-        <v>245.1494</v>
+        <v>201.0006181818182</v>
       </c>
       <c r="X8" t="n">
-        <v>545.6558249999999</v>
+        <v>422.07124</v>
       </c>
       <c r="Y8" t="n">
-        <v>333.262375</v>
+        <v>333.89877</v>
       </c>
       <c r="Z8" t="n">
-        <v>374.72955</v>
+        <v>371.9048666666666</v>
       </c>
       <c r="AA8" t="n">
-        <v>446.924425</v>
+        <v>444.1260333333333</v>
       </c>
       <c r="AB8" t="n">
-        <v>724.74225</v>
+        <v>550.2894111111111</v>
       </c>
       <c r="AC8" t="n">
-        <v>404.103775</v>
+        <v>402.7091666666667</v>
       </c>
       <c r="AD8" t="n">
-        <v>471.075025</v>
+        <v>442.0611</v>
       </c>
       <c r="AE8" t="n">
-        <v>353.401825</v>
+        <v>358.4031222222222</v>
       </c>
       <c r="AF8" t="n">
-        <v>964935.3825000001</v>
+        <v>587448.5988888888</v>
       </c>
       <c r="AG8" t="n">
         <v>10</v>
@@ -1310,94 +1310,94 @@
         <v>40</v>
       </c>
       <c r="C9" t="n">
-        <v>443865361.308</v>
+        <v>159425486.9385714</v>
       </c>
       <c r="D9" t="n">
-        <v>2279027.75</v>
+        <v>2150394.923076923</v>
       </c>
       <c r="E9" t="n">
-        <v>1046.64832475</v>
+        <v>684.9006790769231</v>
       </c>
       <c r="F9" t="n">
-        <v>32.8255975</v>
+        <v>14.28534246153846</v>
       </c>
       <c r="G9" t="n">
-        <v>34.8062175</v>
+        <v>38.45657538461538</v>
       </c>
       <c r="H9" t="n">
-        <v>19.01653975</v>
+        <v>20.99530284615385</v>
       </c>
       <c r="I9" t="n">
-        <v>68.48983749999999</v>
+        <v>57.1197025</v>
       </c>
       <c r="J9" t="n">
-        <v>41.1929825</v>
+        <v>33.64068416666667</v>
       </c>
       <c r="K9" t="n">
-        <v>79.5680215</v>
+        <v>91.17454624999999</v>
       </c>
       <c r="L9" t="n">
-        <v>1233.553325</v>
+        <v>1096.239675</v>
       </c>
       <c r="M9" t="n">
-        <v>196.9380575</v>
+        <v>118.7777608333333</v>
       </c>
       <c r="N9" t="n">
-        <v>3000729.925</v>
+        <v>2997006.272727273</v>
       </c>
       <c r="O9" t="n">
-        <v>36222.7925</v>
+        <v>15551.46645454545</v>
       </c>
       <c r="P9" t="n">
-        <v>97.9876075</v>
+        <v>382.0209354545455</v>
       </c>
       <c r="Q9" t="n">
-        <v>695.8818699999999</v>
+        <v>2298.153634545455</v>
       </c>
       <c r="R9" t="n">
-        <v>187.2208</v>
+        <v>173.236616</v>
       </c>
       <c r="S9" t="n">
-        <v>79.69259</v>
+        <v>130.0280145454545</v>
       </c>
       <c r="T9" t="n">
-        <v>38978.6875</v>
+        <v>24661.05754545455</v>
       </c>
       <c r="U9" t="n">
-        <v>405.1008125</v>
+        <v>55471.76072272727</v>
       </c>
       <c r="V9" t="n">
-        <v>97.1835975</v>
+        <v>119.0406845454545</v>
       </c>
       <c r="W9" t="n">
-        <v>245.13755</v>
+        <v>200.7663090909091</v>
       </c>
       <c r="X9" t="n">
-        <v>532.579025</v>
+        <v>416.51452</v>
       </c>
       <c r="Y9" t="n">
-        <v>331.58485</v>
+        <v>332.68578</v>
       </c>
       <c r="Z9" t="n">
-        <v>374.15165</v>
+        <v>371.0761</v>
       </c>
       <c r="AA9" t="n">
-        <v>446.8985</v>
+        <v>443.3306333333333</v>
       </c>
       <c r="AB9" t="n">
-        <v>718.19475</v>
+        <v>544.3057444444444</v>
       </c>
       <c r="AC9" t="n">
-        <v>403.904975</v>
+        <v>402.0436888888889</v>
       </c>
       <c r="AD9" t="n">
-        <v>470.687725</v>
+        <v>439.2446</v>
       </c>
       <c r="AE9" t="n">
-        <v>325.21165</v>
+        <v>345.6946222222222</v>
       </c>
       <c r="AF9" t="n">
-        <v>879534.46</v>
+        <v>527649.8466666667</v>
       </c>
       <c r="AG9" t="n">
         <v>10</v>
@@ -1411,94 +1411,94 @@
         <v>50</v>
       </c>
       <c r="C10" t="n">
-        <v>377807202.65</v>
+        <v>135635839.5492857</v>
       </c>
       <c r="D10" t="n">
-        <v>2075631.25</v>
+        <v>1144349.538461538</v>
       </c>
       <c r="E10" t="n">
-        <v>946.130560525</v>
+        <v>583.2879211615384</v>
       </c>
       <c r="F10" t="n">
-        <v>32.8140475</v>
+        <v>14.10893423076923</v>
       </c>
       <c r="G10" t="n">
-        <v>34.01003</v>
+        <v>36.28811538461538</v>
       </c>
       <c r="H10" t="n">
-        <v>18.11190225</v>
+        <v>19.99174761538461</v>
       </c>
       <c r="I10" t="n">
-        <v>64.82969750000001</v>
+        <v>53.99659833333334</v>
       </c>
       <c r="J10" t="n">
-        <v>40.388235</v>
+        <v>33.23077333333333</v>
       </c>
       <c r="K10" t="n">
-        <v>74.78090575</v>
+        <v>87.341469</v>
       </c>
       <c r="L10" t="n">
-        <v>1164.162475</v>
+        <v>1056.401141666667</v>
       </c>
       <c r="M10" t="n">
-        <v>190.9083575</v>
+        <v>110.9644725</v>
       </c>
       <c r="N10" t="n">
-        <v>2921967.175</v>
+        <v>2934521.6</v>
       </c>
       <c r="O10" t="n">
-        <v>36222.7925</v>
+        <v>15511.70691818182</v>
       </c>
       <c r="P10" t="n">
-        <v>84.5967725</v>
+        <v>157.1201618181818</v>
       </c>
       <c r="Q10" t="n">
-        <v>649.6178199999999</v>
+        <v>2261.907179090909</v>
       </c>
       <c r="R10" t="n">
-        <v>182.89045</v>
+        <v>151.4320941818182</v>
       </c>
       <c r="S10" t="n">
-        <v>70.4391675</v>
+        <v>126.2948372727273</v>
       </c>
       <c r="T10" t="n">
-        <v>38858.2325</v>
+        <v>24455.59763636364</v>
       </c>
       <c r="U10" t="n">
-        <v>402.55052</v>
+        <v>47393.62016181819</v>
       </c>
       <c r="V10" t="n">
-        <v>95.31187250000001</v>
+        <v>118.0546090909091</v>
       </c>
       <c r="W10" t="n">
-        <v>243.265475</v>
+        <v>168.5696909090909</v>
       </c>
       <c r="X10" t="n">
-        <v>530.0585</v>
+        <v>415.36712</v>
       </c>
       <c r="Y10" t="n">
-        <v>330.839875</v>
+        <v>332.06024</v>
       </c>
       <c r="Z10" t="n">
-        <v>374.13615</v>
+        <v>371.0072777777778</v>
       </c>
       <c r="AA10" t="n">
-        <v>446.131825</v>
+        <v>442.9221888888889</v>
       </c>
       <c r="AB10" t="n">
-        <v>718.1513</v>
+        <v>529.8559555555555</v>
       </c>
       <c r="AC10" t="n">
-        <v>403.872875</v>
+        <v>401.7818111111111</v>
       </c>
       <c r="AD10" t="n">
-        <v>464.8558</v>
+        <v>435.6167444444444</v>
       </c>
       <c r="AE10" t="n">
-        <v>320.004825</v>
+        <v>340.9179777777778</v>
       </c>
       <c r="AF10" t="n">
-        <v>876226.6775</v>
+        <v>516982.1477777778</v>
       </c>
       <c r="AG10" t="n">
         <v>10</v>
@@ -1512,94 +1512,94 @@
         <v>60</v>
       </c>
       <c r="C11" t="n">
-        <v>355647723.092</v>
+        <v>127681696.7714286</v>
       </c>
       <c r="D11" t="n">
-        <v>543477.25</v>
+        <v>410979.6153846154</v>
       </c>
       <c r="E11" t="n">
-        <v>946.122527175</v>
+        <v>551.220113976923</v>
       </c>
       <c r="F11" t="n">
-        <v>32.35203525</v>
+        <v>13.92537961538462</v>
       </c>
       <c r="G11" t="n">
-        <v>33.9231775</v>
+        <v>35.26758384615385</v>
       </c>
       <c r="H11" t="n">
-        <v>17.824638</v>
+        <v>19.52324653846154</v>
       </c>
       <c r="I11" t="n">
-        <v>60.359655</v>
+        <v>52.35961666666666</v>
       </c>
       <c r="J11" t="n">
-        <v>39.92252</v>
+        <v>32.9484325</v>
       </c>
       <c r="K11" t="n">
-        <v>73.73945175</v>
+        <v>79.64935266666667</v>
       </c>
       <c r="L11" t="n">
-        <v>934.830875</v>
+        <v>978.5874916666667</v>
       </c>
       <c r="M11" t="n">
-        <v>190.2874975</v>
+        <v>108.4901358333333</v>
       </c>
       <c r="N11" t="n">
-        <v>2916684.175</v>
+        <v>2915014.381818182</v>
       </c>
       <c r="O11" t="n">
-        <v>36222.7925</v>
+        <v>15511.70691818182</v>
       </c>
       <c r="P11" t="n">
-        <v>84.5967725</v>
+        <v>157.1201618181818</v>
       </c>
       <c r="Q11" t="n">
-        <v>622.199445</v>
+        <v>2207.597879090909</v>
       </c>
       <c r="R11" t="n">
-        <v>168.460375</v>
+        <v>142.9560223636364</v>
       </c>
       <c r="S11" t="n">
-        <v>61.62718750000001</v>
+        <v>122.9780972727273</v>
       </c>
       <c r="T11" t="n">
-        <v>35658.27</v>
+        <v>23219.22672727273</v>
       </c>
       <c r="U11" t="n">
-        <v>320.272685</v>
+        <v>43977.65254909091</v>
       </c>
       <c r="V11" t="n">
-        <v>94.9240975</v>
+        <v>117.7459772727273</v>
       </c>
       <c r="W11" t="n">
-        <v>239.65185</v>
+        <v>164.4579454545454</v>
       </c>
       <c r="X11" t="n">
-        <v>530.04945</v>
+        <v>414.8654500000001</v>
       </c>
       <c r="Y11" t="n">
-        <v>330.29745</v>
+        <v>331.56274</v>
       </c>
       <c r="Z11" t="n">
-        <v>370.96755</v>
+        <v>369.5502</v>
       </c>
       <c r="AA11" t="n">
-        <v>446.131825</v>
+        <v>442.5035222222222</v>
       </c>
       <c r="AB11" t="n">
-        <v>694.9485999999999</v>
+        <v>515.7951222222223</v>
       </c>
       <c r="AC11" t="n">
-        <v>403.3627</v>
+        <v>400.7604111111111</v>
       </c>
       <c r="AD11" t="n">
-        <v>464.624125</v>
+        <v>434.7879444444445</v>
       </c>
       <c r="AE11" t="n">
-        <v>309.8504</v>
+        <v>334.9599111111111</v>
       </c>
       <c r="AF11" t="n">
-        <v>705427.6949999999</v>
+        <v>439905.0177777777</v>
       </c>
       <c r="AG11" t="n">
         <v>10</v>
@@ -1613,94 +1613,94 @@
         <v>70</v>
       </c>
       <c r="C12" t="n">
-        <v>355647723.092</v>
+        <v>127626425.9342857</v>
       </c>
       <c r="D12" t="n">
-        <v>543477.25</v>
+        <v>318529.3846153846</v>
       </c>
       <c r="E12" t="n">
-        <v>920.79071514</v>
+        <v>522.6476818123076</v>
       </c>
       <c r="F12" t="n">
-        <v>32.34827275</v>
+        <v>13.72569123076923</v>
       </c>
       <c r="G12" t="n">
-        <v>33.70363</v>
+        <v>35.00140153846154</v>
       </c>
       <c r="H12" t="n">
-        <v>11.9818235</v>
+        <v>15.67842308333333</v>
       </c>
       <c r="I12" t="n">
-        <v>60.338645</v>
+        <v>52.01368249999999</v>
       </c>
       <c r="J12" t="n">
-        <v>39.92234</v>
+        <v>32.81731666666666</v>
       </c>
       <c r="K12" t="n">
-        <v>73.727318</v>
+        <v>77.20553725000001</v>
       </c>
       <c r="L12" t="n">
-        <v>934.797225</v>
+        <v>976.9282416666666</v>
       </c>
       <c r="M12" t="n">
-        <v>189.3899725</v>
+        <v>106.9363541666667</v>
       </c>
       <c r="N12" t="n">
-        <v>2897719.175</v>
+        <v>2789372.354545454</v>
       </c>
       <c r="O12" t="n">
-        <v>36222.7925</v>
+        <v>15511.70691818182</v>
       </c>
       <c r="P12" t="n">
-        <v>81.78419249999999</v>
+        <v>155.7819754545454</v>
       </c>
       <c r="Q12" t="n">
-        <v>621.5833625</v>
+        <v>2207.190258181818</v>
       </c>
       <c r="R12" t="n">
-        <v>156.62011</v>
+        <v>137.6104341818182</v>
       </c>
       <c r="S12" t="n">
-        <v>60.4250975</v>
+        <v>122.1463127272727</v>
       </c>
       <c r="T12" t="n">
-        <v>35658.27</v>
+        <v>23219.22672727273</v>
       </c>
       <c r="U12" t="n">
-        <v>256.600755</v>
+        <v>42804.57130181819</v>
       </c>
       <c r="V12" t="n">
-        <v>94.9240975</v>
+        <v>117.6938863636364</v>
       </c>
       <c r="W12" t="n">
-        <v>239.5252</v>
+        <v>152.8005</v>
       </c>
       <c r="X12" t="n">
-        <v>530.04855</v>
+        <v>414.50336</v>
       </c>
       <c r="Y12" t="n">
-        <v>329.257175</v>
+        <v>331.03273</v>
       </c>
       <c r="Z12" t="n">
-        <v>361.5284</v>
+        <v>365.1044555555556</v>
       </c>
       <c r="AA12" t="n">
-        <v>442.664225</v>
+        <v>440.8610888888889</v>
       </c>
       <c r="AB12" t="n">
-        <v>694.94675</v>
+        <v>514.4141999999999</v>
       </c>
       <c r="AC12" t="n">
-        <v>403.361925</v>
+        <v>400.6290555555556</v>
       </c>
       <c r="AD12" t="n">
-        <v>464.384625</v>
+        <v>403.0278444444444</v>
       </c>
       <c r="AE12" t="n">
-        <v>308.787025</v>
+        <v>334.2682777777778</v>
       </c>
       <c r="AF12" t="n">
-        <v>698837.5125</v>
+        <v>430799.6166666666</v>
       </c>
       <c r="AG12" t="n">
         <v>10</v>
@@ -1714,94 +1714,94 @@
         <v>80</v>
       </c>
       <c r="C13" t="n">
-        <v>355647671.6</v>
+        <v>127608845.4514286</v>
       </c>
       <c r="D13" t="n">
-        <v>542022</v>
+        <v>309374.1538461539</v>
       </c>
       <c r="E13" t="n">
-        <v>920.7842566575</v>
+        <v>483.3924014330769</v>
       </c>
       <c r="F13" t="n">
-        <v>32.34200525</v>
+        <v>13.643939</v>
       </c>
       <c r="G13" t="n">
-        <v>33.5700575</v>
+        <v>34.57970846153846</v>
       </c>
       <c r="H13" t="n">
-        <v>11.346316</v>
+        <v>14.9477355</v>
       </c>
       <c r="I13" t="n">
-        <v>60.33798</v>
+        <v>51.91994166666667</v>
       </c>
       <c r="J13" t="n">
-        <v>38.9792775</v>
+        <v>32.46227333333334</v>
       </c>
       <c r="K13" t="n">
-        <v>73.70186074999999</v>
+        <v>75.86360316666666</v>
       </c>
       <c r="L13" t="n">
-        <v>934.7849</v>
+        <v>974.5146166666667</v>
       </c>
       <c r="M13" t="n">
-        <v>129.4982725</v>
+        <v>86.07334583333333</v>
       </c>
       <c r="N13" t="n">
-        <v>2811244.925</v>
+        <v>2747206.709090909</v>
       </c>
       <c r="O13" t="n">
-        <v>36222.16</v>
+        <v>15511.47691818182</v>
       </c>
       <c r="P13" t="n">
-        <v>68.64560499999999</v>
+        <v>150.3899245454545</v>
       </c>
       <c r="Q13" t="n">
-        <v>579.624015</v>
+        <v>2182.686310909091</v>
       </c>
       <c r="R13" t="n">
-        <v>156.06246</v>
+        <v>129.7703332727273</v>
       </c>
       <c r="S13" t="n">
-        <v>53.2920525</v>
+        <v>119.5254945454545</v>
       </c>
       <c r="T13" t="n">
-        <v>35292.89</v>
+        <v>22724.07490909091</v>
       </c>
       <c r="U13" t="n">
-        <v>256.321225</v>
+        <v>40494.74656363636</v>
       </c>
       <c r="V13" t="n">
-        <v>91.04766000000001</v>
+        <v>114.1766663636364</v>
       </c>
       <c r="W13" t="n">
-        <v>237.717125</v>
+        <v>151.8138818181818</v>
       </c>
       <c r="X13" t="n">
-        <v>520.5608</v>
+        <v>410.5725</v>
       </c>
       <c r="Y13" t="n">
-        <v>329.22485</v>
+        <v>331.01806</v>
       </c>
       <c r="Z13" t="n">
-        <v>360.97075</v>
+        <v>364.7080888888889</v>
       </c>
       <c r="AA13" t="n">
-        <v>442.663975</v>
+        <v>440.8475555555555</v>
       </c>
       <c r="AB13" t="n">
-        <v>692.88165</v>
+        <v>512.9963333333333</v>
       </c>
       <c r="AC13" t="n">
-        <v>403.3457</v>
+        <v>400.6015888888889</v>
       </c>
       <c r="AD13" t="n">
-        <v>463.699875</v>
+        <v>402.0917888888889</v>
       </c>
       <c r="AE13" t="n">
-        <v>303.886575</v>
+        <v>331.9515777777777</v>
       </c>
       <c r="AF13" t="n">
-        <v>698837.0475</v>
+        <v>430230.65</v>
       </c>
       <c r="AG13" t="n">
         <v>10</v>
@@ -1815,94 +1815,94 @@
         <v>90</v>
       </c>
       <c r="C14" t="n">
-        <v>237610583.738</v>
+        <v>85431598.94000001</v>
       </c>
       <c r="D14" t="n">
-        <v>524326</v>
+        <v>303749.4615384616</v>
       </c>
       <c r="E14" t="n">
-        <v>920.782640885</v>
+        <v>451.8239642723077</v>
       </c>
       <c r="F14" t="n">
-        <v>32.28477775</v>
+        <v>13.58751846153846</v>
       </c>
       <c r="G14" t="n">
-        <v>33.49910250000001</v>
+        <v>34.50134923076923</v>
       </c>
       <c r="H14" t="n">
-        <v>11.338756</v>
+        <v>13.8282085</v>
       </c>
       <c r="I14" t="n">
-        <v>60.334615</v>
+        <v>51.8504475</v>
       </c>
       <c r="J14" t="n">
-        <v>38.97801</v>
+        <v>32.4042075</v>
       </c>
       <c r="K14" t="n">
-        <v>68.65913499999999</v>
+        <v>71.93241208333333</v>
       </c>
       <c r="L14" t="n">
-        <v>934.7708749999999</v>
+        <v>969.2914833333333</v>
       </c>
       <c r="M14" t="n">
-        <v>122.783685</v>
+        <v>83.10481083333333</v>
       </c>
       <c r="N14" t="n">
-        <v>2798039.925</v>
+        <v>2730459.336363636</v>
       </c>
       <c r="O14" t="n">
-        <v>35441.825</v>
+        <v>15208.78772727273</v>
       </c>
       <c r="P14" t="n">
-        <v>68.59913</v>
+        <v>149.6001336363636</v>
       </c>
       <c r="Q14" t="n">
-        <v>512.865465</v>
+        <v>2156.873838181818</v>
       </c>
       <c r="R14" t="n">
-        <v>155.92346</v>
+        <v>129.4691923636364</v>
       </c>
       <c r="S14" t="n">
-        <v>49.9745575</v>
+        <v>118.3157690909091</v>
       </c>
       <c r="T14" t="n">
-        <v>32603.6425</v>
+        <v>21718.53218181818</v>
       </c>
       <c r="U14" t="n">
-        <v>241.965475</v>
+        <v>38501.39792727272</v>
       </c>
       <c r="V14" t="n">
-        <v>64.48728249999999</v>
+        <v>104.4310109090909</v>
       </c>
       <c r="W14" t="n">
-        <v>237.034275</v>
+        <v>156.33584</v>
       </c>
       <c r="X14" t="n">
-        <v>520.5454999999999</v>
+        <v>410.4195800000001</v>
       </c>
       <c r="Y14" t="n">
-        <v>329.20565</v>
+        <v>330.94887</v>
       </c>
       <c r="Z14" t="n">
-        <v>360.1277</v>
+        <v>364.0721666666666</v>
       </c>
       <c r="AA14" t="n">
-        <v>442.35025</v>
+        <v>440.4784888888889</v>
       </c>
       <c r="AB14" t="n">
-        <v>690.7056</v>
+        <v>511.9877111111111</v>
       </c>
       <c r="AC14" t="n">
-        <v>403.169825</v>
+        <v>400.5133777777777</v>
       </c>
       <c r="AD14" t="n">
-        <v>452.637175</v>
+        <v>396.6006222222222</v>
       </c>
       <c r="AE14" t="n">
-        <v>303.88625</v>
+        <v>331.3231</v>
       </c>
       <c r="AF14" t="n">
-        <v>698819.8625</v>
+        <v>428933.07</v>
       </c>
       <c r="AG14" t="n">
         <v>10</v>
@@ -1916,94 +1916,94 @@
         <v>100</v>
       </c>
       <c r="C15" t="n">
-        <v>237608666.73</v>
+        <v>85430914.2942857</v>
       </c>
       <c r="D15" t="n">
-        <v>523872.25</v>
+        <v>252005.6153846154</v>
       </c>
       <c r="E15" t="n">
-        <v>870.57620893275</v>
+        <v>422.9317929023846</v>
       </c>
       <c r="F15" t="n">
-        <v>28.08489025</v>
+        <v>12.22614653846154</v>
       </c>
       <c r="G15" t="n">
-        <v>29.3117475</v>
+        <v>33.19731384615385</v>
       </c>
       <c r="H15" t="n">
-        <v>11.338446</v>
+        <v>13.665811</v>
       </c>
       <c r="I15" t="n">
-        <v>60.32916</v>
+        <v>51.79287249999999</v>
       </c>
       <c r="J15" t="n">
-        <v>38.975895</v>
+        <v>32.4035025</v>
       </c>
       <c r="K15" t="n">
-        <v>68.6494355</v>
+        <v>70.90162891666667</v>
       </c>
       <c r="L15" t="n">
-        <v>934.767325</v>
+        <v>969.0876499999999</v>
       </c>
       <c r="M15" t="n">
-        <v>122.693655</v>
+        <v>82.5850325</v>
       </c>
       <c r="N15" t="n">
-        <v>2794531.875</v>
+        <v>2728739.490909091</v>
       </c>
       <c r="O15" t="n">
-        <v>35441.825</v>
+        <v>15208.78772727273</v>
       </c>
       <c r="P15" t="n">
-        <v>68.5678875</v>
+        <v>149.5887727272727</v>
       </c>
       <c r="Q15" t="n">
-        <v>394.667015</v>
+        <v>2113.892583636363</v>
       </c>
       <c r="R15" t="n">
-        <v>155.599685</v>
+        <v>128.7637923636364</v>
       </c>
       <c r="S15" t="n">
-        <v>49.7141</v>
+        <v>118.2210572727273</v>
       </c>
       <c r="T15" t="n">
-        <v>31514.995</v>
+        <v>21308.13763636364</v>
       </c>
       <c r="U15" t="n">
-        <v>238.732475</v>
+        <v>36287.82229090909</v>
       </c>
       <c r="V15" t="n">
-        <v>64.4072575</v>
+        <v>103.8916009090909</v>
       </c>
       <c r="W15" t="n">
-        <v>237.0319</v>
+        <v>156.24318</v>
       </c>
       <c r="X15" t="n">
-        <v>520.543425</v>
+        <v>410.3739899999999</v>
       </c>
       <c r="Y15" t="n">
-        <v>328.28975</v>
+        <v>330.57735</v>
       </c>
       <c r="Z15" t="n">
-        <v>357.24205</v>
+        <v>362.7794333333334</v>
       </c>
       <c r="AA15" t="n">
-        <v>441.8738</v>
+        <v>440.2287777777777</v>
       </c>
       <c r="AB15" t="n">
-        <v>690.704375</v>
+        <v>511.8823222222222</v>
       </c>
       <c r="AC15" t="n">
-        <v>403.076625</v>
+        <v>400.4606666666666</v>
       </c>
       <c r="AD15" t="n">
-        <v>448.54445</v>
+        <v>394.7436333333333</v>
       </c>
       <c r="AE15" t="n">
-        <v>303.40885</v>
+        <v>331.1109222222222</v>
       </c>
       <c r="AF15" t="n">
-        <v>530403.14</v>
+        <v>354081.1933333333</v>
       </c>
       <c r="AG15" t="n">
         <v>10</v>

</xml_diff>

<commit_message>
Memetic version using ARO as Local Search
</commit_message>
<xml_diff>
--- a/cec2017real-master/code/results_ARO/results_cec2017_10.xlsx
+++ b/cec2017real-master/code/results_ARO/results_cec2017_10.xlsx
@@ -603,94 +603,94 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>4939910110.555555</v>
+        <v>139527700</v>
       </c>
       <c r="D2" t="n">
-        <v>3.973261253675272e+20</v>
+        <v>23183600</v>
       </c>
       <c r="E2" t="n">
-        <v>28842.17266666667</v>
+        <v>27832.08</v>
       </c>
       <c r="F2" t="n">
-        <v>421.31041775</v>
+        <v>58.29218</v>
       </c>
       <c r="G2" t="n">
-        <v>72.24009208333334</v>
+        <v>65.77184</v>
       </c>
       <c r="H2" t="n">
-        <v>46.48655</v>
+        <v>44.51387</v>
       </c>
       <c r="I2" t="n">
-        <v>177.1539381818182</v>
+        <v>58.84726</v>
       </c>
       <c r="J2" t="n">
-        <v>86.57117272727272</v>
+        <v>57.79195</v>
       </c>
       <c r="K2" t="n">
-        <v>1366.303177272727</v>
+        <v>1015.923</v>
       </c>
       <c r="L2" t="n">
-        <v>1663.922614285714</v>
+        <v>2067.102</v>
       </c>
       <c r="M2" t="n">
-        <v>2129.762557142857</v>
+        <v>142.9139</v>
       </c>
       <c r="N2" t="n">
-        <v>150453589.3809524</v>
+        <v>26017340</v>
       </c>
       <c r="O2" t="n">
-        <v>16301727.1414</v>
+        <v>34452.05</v>
       </c>
       <c r="P2" t="n">
-        <v>8695.488905</v>
+        <v>26994.75</v>
       </c>
       <c r="Q2" t="n">
-        <v>111120.1867</v>
+        <v>20418.91</v>
       </c>
       <c r="R2" t="n">
-        <v>521.64437</v>
+        <v>187.301</v>
       </c>
       <c r="S2" t="n">
-        <v>302.698475</v>
+        <v>100.0355</v>
       </c>
       <c r="T2" t="n">
-        <v>19864179.651</v>
+        <v>32675.47</v>
       </c>
       <c r="U2" t="n">
-        <v>8847991.194975</v>
+        <v>5561.391</v>
       </c>
       <c r="V2" t="n">
-        <v>266.08273</v>
+        <v>49.95555</v>
       </c>
       <c r="W2" t="n">
-        <v>291.267145</v>
+        <v>241.9165</v>
       </c>
       <c r="X2" t="n">
-        <v>886.2493210526314</v>
+        <v>222.7606</v>
       </c>
       <c r="Y2" t="n">
-        <v>436.2236210526316</v>
+        <v>378.7792</v>
       </c>
       <c r="Z2" t="n">
-        <v>414.1032</v>
+        <v>380.5803</v>
       </c>
       <c r="AA2" t="n">
-        <v>1402.841011111111</v>
+        <v>504.155</v>
       </c>
       <c r="AB2" t="n">
-        <v>1132.025333333333</v>
+        <v>634.6195</v>
       </c>
       <c r="AC2" t="n">
-        <v>721.6423388888888</v>
+        <v>409.1311</v>
       </c>
       <c r="AD2" t="n">
-        <v>746.9042777777778</v>
+        <v>590.2116</v>
       </c>
       <c r="AE2" t="n">
-        <v>584.0653555555556</v>
+        <v>377.7764</v>
       </c>
       <c r="AF2" t="n">
-        <v>2621326.977777778</v>
+        <v>3593601</v>
       </c>
       <c r="AG2" t="n">
         <v>10</v>
@@ -704,94 +704,94 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>3278705520.085714</v>
+        <v>6074745</v>
       </c>
       <c r="D3" t="n">
-        <v>3.973261251188563e+20</v>
+        <v>2389364</v>
       </c>
       <c r="E3" t="n">
-        <v>20411.87566666667</v>
+        <v>19292.27</v>
       </c>
       <c r="F3" t="n">
-        <v>321.336016</v>
+        <v>18.50758</v>
       </c>
       <c r="G3" t="n">
-        <v>65.3103725</v>
+        <v>38.16961</v>
       </c>
       <c r="H3" t="n">
-        <v>37.6835625</v>
+        <v>39.73399</v>
       </c>
       <c r="I3" t="n">
-        <v>139.6903445454546</v>
+        <v>58.84726</v>
       </c>
       <c r="J3" t="n">
-        <v>68.51216272727272</v>
+        <v>31.37164</v>
       </c>
       <c r="K3" t="n">
-        <v>941.5013218181819</v>
+        <v>1015.923</v>
       </c>
       <c r="L3" t="n">
-        <v>1529.970009523809</v>
+        <v>1232.983</v>
       </c>
       <c r="M3" t="n">
-        <v>1250.076965714286</v>
+        <v>61.97694</v>
       </c>
       <c r="N3" t="n">
-        <v>109411900.4285714</v>
+        <v>2931255</v>
       </c>
       <c r="O3" t="n">
-        <v>1041384.75795</v>
+        <v>31401.88</v>
       </c>
       <c r="P3" t="n">
-        <v>7624.367459999999</v>
+        <v>16466.87</v>
       </c>
       <c r="Q3" t="n">
-        <v>57555.2031</v>
+        <v>20305.59</v>
       </c>
       <c r="R3" t="n">
-        <v>419.20121</v>
+        <v>158.1203</v>
       </c>
       <c r="S3" t="n">
-        <v>231.8909395</v>
+        <v>55.44457</v>
       </c>
       <c r="T3" t="n">
-        <v>13559312.448</v>
+        <v>32675.47</v>
       </c>
       <c r="U3" t="n">
-        <v>105682.496325</v>
+        <v>4639.433</v>
       </c>
       <c r="V3" t="n">
-        <v>214.6347465</v>
+        <v>38.36337</v>
       </c>
       <c r="W3" t="n">
-        <v>271.58984</v>
+        <v>232.3665</v>
       </c>
       <c r="X3" t="n">
-        <v>781.8117052631579</v>
+        <v>124.0848</v>
       </c>
       <c r="Y3" t="n">
-        <v>362.8438368421052</v>
+        <v>367.2743</v>
       </c>
       <c r="Z3" t="n">
-        <v>405.9645368421053</v>
+        <v>357.2267</v>
       </c>
       <c r="AA3" t="n">
-        <v>672.1728444444444</v>
+        <v>452.3694</v>
       </c>
       <c r="AB3" t="n">
-        <v>977.5296888888889</v>
+        <v>359.8505</v>
       </c>
       <c r="AC3" t="n">
-        <v>425.9266666666667</v>
+        <v>394.2179</v>
       </c>
       <c r="AD3" t="n">
-        <v>712.739588888889</v>
+        <v>589.8894</v>
       </c>
       <c r="AE3" t="n">
-        <v>476.7529</v>
+        <v>324.2979</v>
       </c>
       <c r="AF3" t="n">
-        <v>1508942.988888889</v>
+        <v>2116162</v>
       </c>
       <c r="AG3" t="n">
         <v>10</v>
@@ -805,94 +805,94 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>2183005273.25</v>
+        <v>6074745</v>
       </c>
       <c r="D4" t="n">
-        <v>3.973261250579024e+20</v>
+        <v>2389364</v>
       </c>
       <c r="E4" t="n">
-        <v>16002.96758333333</v>
+        <v>19292.27</v>
       </c>
       <c r="F4" t="n">
-        <v>224.9732597083333</v>
+        <v>18.50758</v>
       </c>
       <c r="G4" t="n">
-        <v>59.72083208333333</v>
+        <v>32.47775</v>
       </c>
       <c r="H4" t="n">
-        <v>32.35697041666666</v>
+        <v>26.92601</v>
       </c>
       <c r="I4" t="n">
-        <v>129.1578177272727</v>
+        <v>58.84726</v>
       </c>
       <c r="J4" t="n">
-        <v>61.85062772727272</v>
+        <v>23.17225</v>
       </c>
       <c r="K4" t="n">
-        <v>731.3756168181818</v>
+        <v>955.5734</v>
       </c>
       <c r="L4" t="n">
-        <v>1475.437295238095</v>
+        <v>1014.602</v>
       </c>
       <c r="M4" t="n">
-        <v>802.1756242857142</v>
+        <v>61.97694</v>
       </c>
       <c r="N4" t="n">
-        <v>77514869.12857144</v>
+        <v>2931255</v>
       </c>
       <c r="O4" t="n">
-        <v>598710.6065</v>
+        <v>28408.5</v>
       </c>
       <c r="P4" t="n">
-        <v>5251.262414999999</v>
+        <v>9162.98</v>
       </c>
       <c r="Q4" t="n">
-        <v>23852.20565</v>
+        <v>1225.371</v>
       </c>
       <c r="R4" t="n">
-        <v>330.228665</v>
+        <v>157.7215</v>
       </c>
       <c r="S4" t="n">
-        <v>196.761303</v>
+        <v>47.22008</v>
       </c>
       <c r="T4" t="n">
-        <v>7093106.345000001</v>
+        <v>14834.14</v>
       </c>
       <c r="U4" t="n">
-        <v>81867.37964999999</v>
+        <v>1134.119</v>
       </c>
       <c r="V4" t="n">
-        <v>190.287814</v>
+        <v>38.36337</v>
       </c>
       <c r="W4" t="n">
-        <v>249.134275</v>
+        <v>232.3665</v>
       </c>
       <c r="X4" t="n">
-        <v>741.7412684210526</v>
+        <v>114.2913</v>
       </c>
       <c r="Y4" t="n">
-        <v>355.9577789473684</v>
+        <v>347.0667</v>
       </c>
       <c r="Z4" t="n">
-        <v>397.6279444444444</v>
+        <v>357.2267</v>
       </c>
       <c r="AA4" t="n">
-        <v>601.8526444444444</v>
+        <v>452.3694</v>
       </c>
       <c r="AB4" t="n">
-        <v>932.9450111111112</v>
+        <v>359.8505</v>
       </c>
       <c r="AC4" t="n">
-        <v>414.7938555555555</v>
+        <v>394.2179</v>
       </c>
       <c r="AD4" t="n">
-        <v>673.8812666666668</v>
+        <v>585.5724</v>
       </c>
       <c r="AE4" t="n">
-        <v>446.99675</v>
+        <v>305.3397</v>
       </c>
       <c r="AF4" t="n">
-        <v>1401942.238888889</v>
+        <v>676719.7</v>
       </c>
       <c r="AG4" t="n">
         <v>10</v>
@@ -906,94 +906,94 @@
         <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>1444250488.428571</v>
+        <v>6074745</v>
       </c>
       <c r="D5" t="n">
-        <v>3.973261250051428e+20</v>
+        <v>166396</v>
       </c>
       <c r="E5" t="n">
-        <v>11418.72081666667</v>
+        <v>16791.48</v>
       </c>
       <c r="F5" t="n">
-        <v>177.5357057083334</v>
+        <v>7.528812</v>
       </c>
       <c r="G5" t="n">
-        <v>52.64676958333333</v>
+        <v>32.47775</v>
       </c>
       <c r="H5" t="n">
-        <v>28.59100558333333</v>
+        <v>16.69443</v>
       </c>
       <c r="I5" t="n">
-        <v>115.0894645454546</v>
+        <v>39.22143</v>
       </c>
       <c r="J5" t="n">
-        <v>56.55732636363636</v>
+        <v>23.17225</v>
       </c>
       <c r="K5" t="n">
-        <v>517.0466113636364</v>
+        <v>616.0712</v>
       </c>
       <c r="L5" t="n">
-        <v>1358.223747619048</v>
+        <v>1014.602</v>
       </c>
       <c r="M5" t="n">
-        <v>532.3533557142857</v>
+        <v>50.20146</v>
       </c>
       <c r="N5" t="n">
-        <v>41418842.9952381</v>
+        <v>2931255</v>
       </c>
       <c r="O5" t="n">
-        <v>574678.5246499999</v>
+        <v>28408.5</v>
       </c>
       <c r="P5" t="n">
-        <v>2558.54124</v>
+        <v>2964.443</v>
       </c>
       <c r="Q5" t="n">
-        <v>8593.470415</v>
+        <v>999.604</v>
       </c>
       <c r="R5" t="n">
-        <v>298.1623</v>
+        <v>157.7215</v>
       </c>
       <c r="S5" t="n">
-        <v>162.080247</v>
+        <v>47.22008</v>
       </c>
       <c r="T5" t="n">
-        <v>5046063.364949999</v>
+        <v>9430.199000000001</v>
       </c>
       <c r="U5" t="n">
-        <v>71912.951235</v>
+        <v>1134.119</v>
       </c>
       <c r="V5" t="n">
-        <v>167.0267695</v>
+        <v>38.36337</v>
       </c>
       <c r="W5" t="n">
-        <v>226.513015</v>
+        <v>232.3665</v>
       </c>
       <c r="X5" t="n">
-        <v>650.1553263157895</v>
+        <v>111.7443</v>
       </c>
       <c r="Y5" t="n">
-        <v>350.686547368421</v>
+        <v>340.6367</v>
       </c>
       <c r="Z5" t="n">
-        <v>389.7586</v>
+        <v>357.2267</v>
       </c>
       <c r="AA5" t="n">
-        <v>542.2159388888889</v>
+        <v>418.1067</v>
       </c>
       <c r="AB5" t="n">
-        <v>816.9910111111111</v>
+        <v>359.8505</v>
       </c>
       <c r="AC5" t="n">
-        <v>410.7379555555556</v>
+        <v>391.3326</v>
       </c>
       <c r="AD5" t="n">
-        <v>644.0869222222223</v>
+        <v>415.236</v>
       </c>
       <c r="AE5" t="n">
-        <v>408.9320055555556</v>
+        <v>305.3397</v>
       </c>
       <c r="AF5" t="n">
-        <v>1331371.527777778</v>
+        <v>458971.2</v>
       </c>
       <c r="AG5" t="n">
         <v>10</v>
@@ -1007,94 +1007,94 @@
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>1282982758.242857</v>
+        <v>6074745</v>
       </c>
       <c r="D6" t="n">
-        <v>3.973261250050145e+20</v>
+        <v>166396</v>
       </c>
       <c r="E6" t="n">
-        <v>7775.247216250001</v>
+        <v>9010.282999999999</v>
       </c>
       <c r="F6" t="n">
-        <v>132.2595370833334</v>
+        <v>7.528812</v>
       </c>
       <c r="G6" t="n">
-        <v>47.48353125</v>
+        <v>22.46341</v>
       </c>
       <c r="H6" t="n">
-        <v>25.46680041666667</v>
+        <v>9.647335999999999</v>
       </c>
       <c r="I6" t="n">
-        <v>100.3345322727273</v>
+        <v>39.22143</v>
       </c>
       <c r="J6" t="n">
-        <v>50.05842545454546</v>
+        <v>23.17225</v>
       </c>
       <c r="K6" t="n">
-        <v>374.9489056818182</v>
+        <v>117.5735</v>
       </c>
       <c r="L6" t="n">
-        <v>1298.852557142857</v>
+        <v>934.8744</v>
       </c>
       <c r="M6" t="n">
-        <v>367.4045342857142</v>
+        <v>50.20146</v>
       </c>
       <c r="N6" t="n">
-        <v>39599873.03809524</v>
+        <v>530455.5</v>
       </c>
       <c r="O6" t="n">
-        <v>423222.0317</v>
+        <v>14305.34</v>
       </c>
       <c r="P6" t="n">
-        <v>1192.9721</v>
+        <v>142.8895</v>
       </c>
       <c r="Q6" t="n">
-        <v>5993.984305</v>
+        <v>999.604</v>
       </c>
       <c r="R6" t="n">
-        <v>273.6052875</v>
+        <v>157.7215</v>
       </c>
       <c r="S6" t="n">
-        <v>136.9124675</v>
+        <v>47.22008</v>
       </c>
       <c r="T6" t="n">
-        <v>4222356.5202</v>
+        <v>4207.233</v>
       </c>
       <c r="U6" t="n">
-        <v>60858.887445</v>
+        <v>1134.119</v>
       </c>
       <c r="V6" t="n">
-        <v>154.6608855</v>
+        <v>38.36337</v>
       </c>
       <c r="W6" t="n">
-        <v>201.44788</v>
+        <v>219.8273</v>
       </c>
       <c r="X6" t="n">
-        <v>600.9478631578947</v>
+        <v>111.7443</v>
       </c>
       <c r="Y6" t="n">
-        <v>345.5585578947369</v>
+        <v>322.6683</v>
       </c>
       <c r="Z6" t="n">
-        <v>382.6182888888889</v>
+        <v>343.487</v>
       </c>
       <c r="AA6" t="n">
-        <v>502.5382555555555</v>
+        <v>418.1067</v>
       </c>
       <c r="AB6" t="n">
-        <v>763.1451</v>
+        <v>359.8505</v>
       </c>
       <c r="AC6" t="n">
-        <v>406.9165611111111</v>
+        <v>391.3326</v>
       </c>
       <c r="AD6" t="n">
-        <v>550.9786388888889</v>
+        <v>415.236</v>
       </c>
       <c r="AE6" t="n">
-        <v>380.7386333333333</v>
+        <v>305.3397</v>
       </c>
       <c r="AF6" t="n">
-        <v>1085262.361111111</v>
+        <v>392789.9</v>
       </c>
       <c r="AG6" t="n">
         <v>10</v>
@@ -1108,94 +1108,94 @@
         <v>20</v>
       </c>
       <c r="C7" t="n">
-        <v>523445525.54</v>
+        <v>3211263</v>
       </c>
       <c r="D7" t="n">
-        <v>1465671619.166667</v>
+        <v>115235</v>
       </c>
       <c r="E7" t="n">
-        <v>5639.314734083334</v>
+        <v>9010.282999999999</v>
       </c>
       <c r="F7" t="n">
-        <v>96.00829329166667</v>
+        <v>7.528812</v>
       </c>
       <c r="G7" t="n">
-        <v>42.51367833333334</v>
+        <v>19.46536</v>
       </c>
       <c r="H7" t="n">
-        <v>22.58486554166667</v>
+        <v>7.56135</v>
       </c>
       <c r="I7" t="n">
-        <v>91.7776540909091</v>
+        <v>39.22143</v>
       </c>
       <c r="J7" t="n">
-        <v>42.52987818181818</v>
+        <v>18.12363</v>
       </c>
       <c r="K7" t="n">
-        <v>311.6557261818182</v>
+        <v>91.45802999999999</v>
       </c>
       <c r="L7" t="n">
-        <v>1210.4351</v>
+        <v>702.2140000000001</v>
       </c>
       <c r="M7" t="n">
-        <v>198.274106</v>
+        <v>44.65686</v>
       </c>
       <c r="N7" t="n">
-        <v>26883833.08095238</v>
+        <v>346149.9</v>
       </c>
       <c r="O7" t="n">
-        <v>75143.117185</v>
+        <v>6576.151</v>
       </c>
       <c r="P7" t="n">
-        <v>670.8835335</v>
+        <v>112.4737</v>
       </c>
       <c r="Q7" t="n">
-        <v>3815.487802000001</v>
+        <v>602.6459</v>
       </c>
       <c r="R7" t="n">
-        <v>211.1347645</v>
+        <v>109.5457</v>
       </c>
       <c r="S7" t="n">
-        <v>115.0294625</v>
+        <v>47.22008</v>
       </c>
       <c r="T7" t="n">
-        <v>614522.7236500001</v>
+        <v>4207.233</v>
       </c>
       <c r="U7" t="n">
-        <v>41316.25283</v>
+        <v>828.0096</v>
       </c>
       <c r="V7" t="n">
-        <v>135.5345265</v>
+        <v>38.36337</v>
       </c>
       <c r="W7" t="n">
-        <v>187.44234</v>
+        <v>219.8273</v>
       </c>
       <c r="X7" t="n">
-        <v>513.3279473684211</v>
+        <v>111.7443</v>
       </c>
       <c r="Y7" t="n">
-        <v>339.1859473684211</v>
+        <v>322.6683</v>
       </c>
       <c r="Z7" t="n">
-        <v>376.3942333333333</v>
+        <v>343.487</v>
       </c>
       <c r="AA7" t="n">
-        <v>475.1462944444444</v>
+        <v>408.8443</v>
       </c>
       <c r="AB7" t="n">
-        <v>621.4356111111111</v>
+        <v>359.8505</v>
       </c>
       <c r="AC7" t="n">
-        <v>402.7785833333334</v>
+        <v>390.5696</v>
       </c>
       <c r="AD7" t="n">
-        <v>516.2600777777777</v>
+        <v>371.9691</v>
       </c>
       <c r="AE7" t="n">
-        <v>354.1375277777778</v>
+        <v>305.3397</v>
       </c>
       <c r="AF7" t="n">
-        <v>728608.7288888888</v>
+        <v>102889.2</v>
       </c>
       <c r="AG7" t="n">
         <v>10</v>
@@ -1209,94 +1209,94 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>413761611.6852</v>
+        <v>3211263</v>
       </c>
       <c r="D8" t="n">
-        <v>999437161.0833334</v>
+        <v>38823</v>
       </c>
       <c r="E8" t="n">
-        <v>4245.920110229166</v>
+        <v>9010.282999999999</v>
       </c>
       <c r="F8" t="n">
-        <v>68.79932408333333</v>
+        <v>7.528812</v>
       </c>
       <c r="G8" t="n">
-        <v>39.94586333333333</v>
+        <v>16.7629</v>
       </c>
       <c r="H8" t="n">
-        <v>20.62431058333333</v>
+        <v>5.23555</v>
       </c>
       <c r="I8" t="n">
-        <v>84.39469818181819</v>
+        <v>39.22143</v>
       </c>
       <c r="J8" t="n">
-        <v>39.58962409090909</v>
+        <v>14.12866</v>
       </c>
       <c r="K8" t="n">
-        <v>257.3733351363637</v>
+        <v>91.45802999999999</v>
       </c>
       <c r="L8" t="n">
-        <v>1132.402619047619</v>
+        <v>702.2140000000001</v>
       </c>
       <c r="M8" t="n">
-        <v>159.3787798095238</v>
+        <v>33.10888</v>
       </c>
       <c r="N8" t="n">
-        <v>17439132.65</v>
+        <v>318601.3</v>
       </c>
       <c r="O8" t="n">
-        <v>74700.271385</v>
+        <v>6195.053</v>
       </c>
       <c r="P8" t="n">
-        <v>386.629512</v>
+        <v>112.4737</v>
       </c>
       <c r="Q8" t="n">
-        <v>2585.6742715</v>
+        <v>602.6459</v>
       </c>
       <c r="R8" t="n">
-        <v>196.47619365</v>
+        <v>109.5457</v>
       </c>
       <c r="S8" t="n">
-        <v>110.580957</v>
+        <v>37.83339</v>
       </c>
       <c r="T8" t="n">
-        <v>131731.43025</v>
+        <v>3290.659</v>
       </c>
       <c r="U8" t="n">
-        <v>34930.56481249999</v>
+        <v>161.6481</v>
       </c>
       <c r="V8" t="n">
-        <v>118.808335</v>
+        <v>33.53934</v>
       </c>
       <c r="W8" t="n">
-        <v>177.74746</v>
+        <v>122.3551</v>
       </c>
       <c r="X8" t="n">
-        <v>501.3827842105263</v>
+        <v>111.2974</v>
       </c>
       <c r="Y8" t="n">
-        <v>337.6164842105263</v>
+        <v>322.6683</v>
       </c>
       <c r="Z8" t="n">
-        <v>368.5321388888889</v>
+        <v>343.487</v>
       </c>
       <c r="AA8" t="n">
-        <v>446.3866</v>
+        <v>408.8443</v>
       </c>
       <c r="AB8" t="n">
-        <v>577.750361111111</v>
+        <v>350.6729</v>
       </c>
       <c r="AC8" t="n">
-        <v>401.7194222222222</v>
+        <v>390.5696</v>
       </c>
       <c r="AD8" t="n">
-        <v>499.3581277777778</v>
+        <v>371.9492</v>
       </c>
       <c r="AE8" t="n">
-        <v>347.5634166666666</v>
+        <v>289.422</v>
       </c>
       <c r="AF8" t="n">
-        <v>662749.0383333333</v>
+        <v>90796.64999999999</v>
       </c>
       <c r="AG8" t="n">
         <v>10</v>
@@ -1310,94 +1310,94 @@
         <v>40</v>
       </c>
       <c r="C9" t="n">
-        <v>410269044.8056</v>
+        <v>3211263</v>
       </c>
       <c r="D9" t="n">
-        <v>998407108.5416666</v>
+        <v>38823</v>
       </c>
       <c r="E9" t="n">
-        <v>3385.634612583333</v>
+        <v>7149.237</v>
       </c>
       <c r="F9" t="n">
-        <v>65.96024670833333</v>
+        <v>7.528812</v>
       </c>
       <c r="G9" t="n">
-        <v>38.02266333333333</v>
+        <v>15.03891</v>
       </c>
       <c r="H9" t="n">
-        <v>19.64331795833333</v>
+        <v>5.23555</v>
       </c>
       <c r="I9" t="n">
-        <v>76.34546999999999</v>
+        <v>39.22143</v>
       </c>
       <c r="J9" t="n">
-        <v>37.78916318181818</v>
+        <v>14.12866</v>
       </c>
       <c r="K9" t="n">
-        <v>239.9715567727273</v>
+        <v>64.58904</v>
       </c>
       <c r="L9" t="n">
-        <v>1075.4955</v>
+        <v>702.2140000000001</v>
       </c>
       <c r="M9" t="n">
-        <v>135.0356521904762</v>
+        <v>33.10888</v>
       </c>
       <c r="N9" t="n">
-        <v>17082208.4</v>
+        <v>234989.5</v>
       </c>
       <c r="O9" t="n">
-        <v>74114.75469999999</v>
+        <v>3418.569</v>
       </c>
       <c r="P9" t="n">
-        <v>334.9147785</v>
+        <v>112.4737</v>
       </c>
       <c r="Q9" t="n">
-        <v>2401.319249</v>
+        <v>602.6459</v>
       </c>
       <c r="R9" t="n">
-        <v>181.67019125</v>
+        <v>31.13351</v>
       </c>
       <c r="S9" t="n">
-        <v>105.4611755</v>
+        <v>37.83339</v>
       </c>
       <c r="T9" t="n">
-        <v>130466.37945</v>
+        <v>3290.659</v>
       </c>
       <c r="U9" t="n">
-        <v>32461.0842395</v>
+        <v>161.6481</v>
       </c>
       <c r="V9" t="n">
-        <v>115.0835275</v>
+        <v>33.53934</v>
       </c>
       <c r="W9" t="n">
-        <v>176.17769</v>
+        <v>118.1346</v>
       </c>
       <c r="X9" t="n">
-        <v>403.4316578947369</v>
+        <v>111.2974</v>
       </c>
       <c r="Y9" t="n">
-        <v>335.788552631579</v>
+        <v>319.3914</v>
       </c>
       <c r="Z9" t="n">
-        <v>359.0377222222222</v>
+        <v>343.487</v>
       </c>
       <c r="AA9" t="n">
-        <v>441.7733333333333</v>
+        <v>408.8443</v>
       </c>
       <c r="AB9" t="n">
-        <v>568.1760111111112</v>
+        <v>330.7999</v>
       </c>
       <c r="AC9" t="n">
-        <v>400.7154277777778</v>
+        <v>390.5696</v>
       </c>
       <c r="AD9" t="n">
-        <v>481.5626</v>
+        <v>349.632</v>
       </c>
       <c r="AE9" t="n">
-        <v>340.6298777777778</v>
+        <v>289.422</v>
       </c>
       <c r="AF9" t="n">
-        <v>574496.2672222223</v>
+        <v>79545.14999999999</v>
       </c>
       <c r="AG9" t="n">
         <v>10</v>
@@ -1411,94 +1411,94 @@
         <v>50</v>
       </c>
       <c r="C10" t="n">
-        <v>396441204.7916</v>
+        <v>2149306</v>
       </c>
       <c r="D10" t="n">
-        <v>997830120.0833334</v>
+        <v>38823</v>
       </c>
       <c r="E10" t="n">
-        <v>3124.392514129167</v>
+        <v>6473.633</v>
       </c>
       <c r="F10" t="n">
-        <v>56.88833475000001</v>
+        <v>6.464287</v>
       </c>
       <c r="G10" t="n">
-        <v>35.94588541666666</v>
+        <v>15.03891</v>
       </c>
       <c r="H10" t="n">
-        <v>18.88802620833333</v>
+        <v>5.23555</v>
       </c>
       <c r="I10" t="n">
-        <v>73.2316740909091</v>
+        <v>39.22143</v>
       </c>
       <c r="J10" t="n">
-        <v>37.05535909090909</v>
+        <v>14.12866</v>
       </c>
       <c r="K10" t="n">
-        <v>226.6112796190476</v>
+        <v>64.58904</v>
       </c>
       <c r="L10" t="n">
-        <v>1047.950423809524</v>
+        <v>684.3185999999999</v>
       </c>
       <c r="M10" t="n">
-        <v>130.0023552380952</v>
+        <v>14.28396</v>
       </c>
       <c r="N10" t="n">
-        <v>16849800.715</v>
+        <v>234989.5</v>
       </c>
       <c r="O10" t="n">
-        <v>73952.526405</v>
+        <v>3418.569</v>
       </c>
       <c r="P10" t="n">
-        <v>208.9478875</v>
+        <v>112.4737</v>
       </c>
       <c r="Q10" t="n">
-        <v>2144.8485385</v>
+        <v>602.6459</v>
       </c>
       <c r="R10" t="n">
-        <v>167.19405275</v>
+        <v>26.53549</v>
       </c>
       <c r="S10" t="n">
-        <v>101.075507</v>
+        <v>37.83339</v>
       </c>
       <c r="T10" t="n">
-        <v>130171.2935</v>
+        <v>2596.993</v>
       </c>
       <c r="U10" t="n">
-        <v>27954.819606</v>
+        <v>77.1284</v>
       </c>
       <c r="V10" t="n">
-        <v>111.643865</v>
+        <v>33.53934</v>
       </c>
       <c r="W10" t="n">
-        <v>157.77255</v>
+        <v>118.1346</v>
       </c>
       <c r="X10" t="n">
-        <v>400.1666584210527</v>
+        <v>111.2974</v>
       </c>
       <c r="Y10" t="n">
-        <v>335.1774421052631</v>
+        <v>312.5602</v>
       </c>
       <c r="Z10" t="n">
-        <v>357.0858833333334</v>
+        <v>343.487</v>
       </c>
       <c r="AA10" t="n">
-        <v>439.5635444444445</v>
+        <v>408.8443</v>
       </c>
       <c r="AB10" t="n">
-        <v>557.1355444444445</v>
+        <v>330.7999</v>
       </c>
       <c r="AC10" t="n">
-        <v>400.5285666666666</v>
+        <v>390.5696</v>
       </c>
       <c r="AD10" t="n">
-        <v>445.2026333333333</v>
+        <v>349.632</v>
       </c>
       <c r="AE10" t="n">
-        <v>334.0483111111111</v>
+        <v>289.422</v>
       </c>
       <c r="AF10" t="n">
-        <v>563014.9516666667</v>
+        <v>79545.14999999999</v>
       </c>
       <c r="AG10" t="n">
         <v>10</v>
@@ -1512,94 +1512,94 @@
         <v>60</v>
       </c>
       <c r="C11" t="n">
-        <v>391018795.876</v>
+        <v>2149306</v>
       </c>
       <c r="D11" t="n">
-        <v>931729982.3333334</v>
+        <v>38823</v>
       </c>
       <c r="E11" t="n">
-        <v>2911.6694527375</v>
+        <v>3934.651</v>
       </c>
       <c r="F11" t="n">
-        <v>41.72005020833333</v>
+        <v>5.388297</v>
       </c>
       <c r="G11" t="n">
-        <v>34.90323125</v>
+        <v>15.03891</v>
       </c>
       <c r="H11" t="n">
-        <v>18.71815726086957</v>
+        <v>5.23555</v>
       </c>
       <c r="I11" t="n">
-        <v>69.96410181818182</v>
+        <v>39.22143</v>
       </c>
       <c r="J11" t="n">
-        <v>36.71854395454545</v>
+        <v>14.12866</v>
       </c>
       <c r="K11" t="n">
-        <v>214.8455763333333</v>
+        <v>64.58904</v>
       </c>
       <c r="L11" t="n">
-        <v>997.3564380952381</v>
+        <v>625.8274</v>
       </c>
       <c r="M11" t="n">
-        <v>127.4526214285714</v>
+        <v>14.28396</v>
       </c>
       <c r="N11" t="n">
-        <v>16650956.19</v>
+        <v>234989.5</v>
       </c>
       <c r="O11" t="n">
-        <v>56505.331005</v>
+        <v>3418.569</v>
       </c>
       <c r="P11" t="n">
-        <v>207.1934425</v>
+        <v>112.4737</v>
       </c>
       <c r="Q11" t="n">
-        <v>2040.0951635</v>
+        <v>602.6459</v>
       </c>
       <c r="R11" t="n">
-        <v>155.12675325</v>
+        <v>26.53549</v>
       </c>
       <c r="S11" t="n">
-        <v>99.1861195</v>
+        <v>37.83339</v>
       </c>
       <c r="T11" t="n">
-        <v>83754.228</v>
+        <v>2596.993</v>
       </c>
       <c r="U11" t="n">
-        <v>26021.445359</v>
+        <v>77.1284</v>
       </c>
       <c r="V11" t="n">
-        <v>106.7045625</v>
+        <v>33.53934</v>
       </c>
       <c r="W11" t="n">
-        <v>154.815655</v>
+        <v>111.4889</v>
       </c>
       <c r="X11" t="n">
-        <v>398.8767215789474</v>
+        <v>110.8909</v>
       </c>
       <c r="Y11" t="n">
-        <v>332.6911578947369</v>
+        <v>312.164</v>
       </c>
       <c r="Z11" t="n">
-        <v>356.0227722222222</v>
+        <v>343.487</v>
       </c>
       <c r="AA11" t="n">
-        <v>434.5360222222222</v>
+        <v>408.8443</v>
       </c>
       <c r="AB11" t="n">
-        <v>547.9556833333332</v>
+        <v>330.7999</v>
       </c>
       <c r="AC11" t="n">
-        <v>399.8413888888888</v>
+        <v>390.5696</v>
       </c>
       <c r="AD11" t="n">
-        <v>438.6673833333333</v>
+        <v>349.632</v>
       </c>
       <c r="AE11" t="n">
-        <v>328.53995</v>
+        <v>289.422</v>
       </c>
       <c r="AF11" t="n">
-        <v>505201.8277777778</v>
+        <v>51969.3</v>
       </c>
       <c r="AG11" t="n">
         <v>10</v>
@@ -1613,94 +1613,94 @@
         <v>70</v>
       </c>
       <c r="C12" t="n">
-        <v>373882156.2072</v>
+        <v>2149306</v>
       </c>
       <c r="D12" t="n">
-        <v>634409772.75</v>
+        <v>38823</v>
       </c>
       <c r="E12" t="n">
-        <v>2067.796521565</v>
+        <v>3934.651</v>
       </c>
       <c r="F12" t="n">
-        <v>36.35260316666667</v>
+        <v>5.388297</v>
       </c>
       <c r="G12" t="n">
-        <v>34.06798791666667</v>
+        <v>15.03891</v>
       </c>
       <c r="H12" t="n">
-        <v>14.84995054545455</v>
+        <v>5.23555</v>
       </c>
       <c r="I12" t="n">
-        <v>67.53097772727273</v>
+        <v>39.22143</v>
       </c>
       <c r="J12" t="n">
-        <v>36.39065940909091</v>
+        <v>14.12866</v>
       </c>
       <c r="K12" t="n">
-        <v>210.1477708571429</v>
+        <v>64.58904</v>
       </c>
       <c r="L12" t="n">
-        <v>984.6755428571428</v>
+        <v>625.8274</v>
       </c>
       <c r="M12" t="n">
-        <v>126.2099147619048</v>
+        <v>14.28396</v>
       </c>
       <c r="N12" t="n">
-        <v>9293811.625</v>
+        <v>234989.5</v>
       </c>
       <c r="O12" t="n">
-        <v>44654.056905</v>
+        <v>3418.569</v>
       </c>
       <c r="P12" t="n">
-        <v>166.45927</v>
+        <v>112.4737</v>
       </c>
       <c r="Q12" t="n">
-        <v>1915.073722</v>
+        <v>602.6459</v>
       </c>
       <c r="R12" t="n">
-        <v>147.28555575</v>
+        <v>26.53549</v>
       </c>
       <c r="S12" t="n">
-        <v>98.62523999999999</v>
+        <v>37.83339</v>
       </c>
       <c r="T12" t="n">
-        <v>83754.228</v>
+        <v>2596.993</v>
       </c>
       <c r="U12" t="n">
-        <v>25066.3969145</v>
+        <v>77.1284</v>
       </c>
       <c r="V12" t="n">
-        <v>105.064965</v>
+        <v>33.53934</v>
       </c>
       <c r="W12" t="n">
-        <v>147.89254</v>
+        <v>111.4889</v>
       </c>
       <c r="X12" t="n">
-        <v>398.4236131578947</v>
+        <v>110.8909</v>
       </c>
       <c r="Y12" t="n">
-        <v>332.0190210526316</v>
+        <v>312.164</v>
       </c>
       <c r="Z12" t="n">
-        <v>353.0269944444444</v>
+        <v>343.487</v>
       </c>
       <c r="AA12" t="n">
-        <v>432.1608833333333</v>
+        <v>408.8443</v>
       </c>
       <c r="AB12" t="n">
-        <v>546.2907611111111</v>
+        <v>330.7999</v>
       </c>
       <c r="AC12" t="n">
-        <v>399.73655</v>
+        <v>390.5696</v>
       </c>
       <c r="AD12" t="n">
-        <v>417.1122444444445</v>
+        <v>349.632</v>
       </c>
       <c r="AE12" t="n">
-        <v>328.1288277777778</v>
+        <v>289.422</v>
       </c>
       <c r="AF12" t="n">
-        <v>495159.8083333333</v>
+        <v>51969.3</v>
       </c>
       <c r="AG12" t="n">
         <v>10</v>
@@ -1714,94 +1714,94 @@
         <v>80</v>
       </c>
       <c r="C13" t="n">
-        <v>226664725.0568</v>
+        <v>2149306</v>
       </c>
       <c r="D13" t="n">
-        <v>470750580.8333333</v>
+        <v>38823</v>
       </c>
       <c r="E13" t="n">
-        <v>2012.06090052625</v>
+        <v>2209.007</v>
       </c>
       <c r="F13" t="n">
-        <v>31.87741908333334</v>
+        <v>5.388297</v>
       </c>
       <c r="G13" t="n">
-        <v>32.80670958333334</v>
+        <v>15.03891</v>
       </c>
       <c r="H13" t="n">
-        <v>14.0208245</v>
+        <v>5.23555</v>
       </c>
       <c r="I13" t="n">
-        <v>63.53402272727272</v>
+        <v>39.22143</v>
       </c>
       <c r="J13" t="n">
-        <v>35.31034031818182</v>
+        <v>14.12866</v>
       </c>
       <c r="K13" t="n">
-        <v>194.8589493809524</v>
+        <v>64.58904</v>
       </c>
       <c r="L13" t="n">
-        <v>957.3414523809524</v>
+        <v>625.8274</v>
       </c>
       <c r="M13" t="n">
-        <v>92.95797019047619</v>
+        <v>14.28396</v>
       </c>
       <c r="N13" t="n">
-        <v>6694360.98</v>
+        <v>182863.2</v>
       </c>
       <c r="O13" t="n">
-        <v>30922.275705</v>
+        <v>3418.569</v>
       </c>
       <c r="P13" t="n">
-        <v>163.493642</v>
+        <v>112.4737</v>
       </c>
       <c r="Q13" t="n">
-        <v>1823.272316</v>
+        <v>546.3324</v>
       </c>
       <c r="R13" t="n">
-        <v>128.22108625</v>
+        <v>26.53549</v>
       </c>
       <c r="S13" t="n">
-        <v>96.5727375</v>
+        <v>37.83339</v>
       </c>
       <c r="T13" t="n">
-        <v>82318.291</v>
+        <v>2596.993</v>
       </c>
       <c r="U13" t="n">
-        <v>23669.8086485</v>
+        <v>77.1284</v>
       </c>
       <c r="V13" t="n">
-        <v>102.954563</v>
+        <v>33.53934</v>
       </c>
       <c r="W13" t="n">
-        <v>137.021005</v>
+        <v>111.4889</v>
       </c>
       <c r="X13" t="n">
-        <v>396.0880931578948</v>
+        <v>110.8909</v>
       </c>
       <c r="Y13" t="n">
-        <v>331.2670473684211</v>
+        <v>312.164</v>
       </c>
       <c r="Z13" t="n">
-        <v>352.0203166666667</v>
+        <v>343.487</v>
       </c>
       <c r="AA13" t="n">
-        <v>431.6757166666667</v>
+        <v>408.8443</v>
       </c>
       <c r="AB13" t="n">
-        <v>524.05055</v>
+        <v>330.7999</v>
       </c>
       <c r="AC13" t="n">
-        <v>399.5585777777778</v>
+        <v>390.5696</v>
       </c>
       <c r="AD13" t="n">
-        <v>414.9249166666667</v>
+        <v>349.632</v>
       </c>
       <c r="AE13" t="n">
-        <v>323.8090166666667</v>
+        <v>289.422</v>
       </c>
       <c r="AF13" t="n">
-        <v>476646.4555555555</v>
+        <v>51969.3</v>
       </c>
       <c r="AG13" t="n">
         <v>10</v>
@@ -1815,94 +1815,94 @@
         <v>90</v>
       </c>
       <c r="C14" t="n">
-        <v>114706693.1304</v>
+        <v>2149306</v>
       </c>
       <c r="D14" t="n">
-        <v>470747534.125</v>
+        <v>38823</v>
       </c>
       <c r="E14" t="n">
-        <v>1675.3784516475</v>
+        <v>2209.007</v>
       </c>
       <c r="F14" t="n">
-        <v>31.83815608333333</v>
+        <v>5.388297</v>
       </c>
       <c r="G14" t="n">
-        <v>31.67781666666667</v>
+        <v>15.03891</v>
       </c>
       <c r="H14" t="n">
-        <v>13.41017340909091</v>
+        <v>4.079457</v>
       </c>
       <c r="I14" t="n">
-        <v>59.04057</v>
+        <v>39.22143</v>
       </c>
       <c r="J14" t="n">
-        <v>35.27866804545454</v>
+        <v>14.12866</v>
       </c>
       <c r="K14" t="n">
-        <v>181.0118457619048</v>
+        <v>11.78862</v>
       </c>
       <c r="L14" t="n">
-        <v>954.3568047619049</v>
+        <v>625.8274</v>
       </c>
       <c r="M14" t="n">
-        <v>77.37858542857143</v>
+        <v>14.28396</v>
       </c>
       <c r="N14" t="n">
-        <v>6685149.925</v>
+        <v>182863.2</v>
       </c>
       <c r="O14" t="n">
-        <v>16765.94915</v>
+        <v>3418.569</v>
       </c>
       <c r="P14" t="n">
-        <v>163.059257</v>
+        <v>112.4737</v>
       </c>
       <c r="Q14" t="n">
-        <v>1781.115876</v>
+        <v>546.3324</v>
       </c>
       <c r="R14" t="n">
-        <v>128.05545875</v>
+        <v>26.53549</v>
       </c>
       <c r="S14" t="n">
-        <v>93.66388499999999</v>
+        <v>37.83339</v>
       </c>
       <c r="T14" t="n">
-        <v>81765.24249999999</v>
+        <v>2596.993</v>
       </c>
       <c r="U14" t="n">
-        <v>22188.6816085</v>
+        <v>77.1284</v>
       </c>
       <c r="V14" t="n">
-        <v>97.5944525</v>
+        <v>33.53934</v>
       </c>
       <c r="W14" t="n">
-        <v>134.3538526315789</v>
+        <v>111.4889</v>
       </c>
       <c r="X14" t="n">
-        <v>396.0076089473685</v>
+        <v>110.8909</v>
       </c>
       <c r="Y14" t="n">
-        <v>330.7953</v>
+        <v>312.164</v>
       </c>
       <c r="Z14" t="n">
-        <v>351.7023555555555</v>
+        <v>343.487</v>
       </c>
       <c r="AA14" t="n">
-        <v>430.3041611111111</v>
+        <v>406.1602</v>
       </c>
       <c r="AB14" t="n">
-        <v>523.5318611111111</v>
+        <v>315.3383</v>
       </c>
       <c r="AC14" t="n">
-        <v>398.9310944444444</v>
+        <v>390.5696</v>
       </c>
       <c r="AD14" t="n">
-        <v>411.9422444444444</v>
+        <v>349.632</v>
       </c>
       <c r="AE14" t="n">
-        <v>318.727</v>
+        <v>289.422</v>
       </c>
       <c r="AF14" t="n">
-        <v>474795.96</v>
+        <v>51969.3</v>
       </c>
       <c r="AG14" t="n">
         <v>10</v>
@@ -1916,94 +1916,94 @@
         <v>100</v>
       </c>
       <c r="C15" t="n">
-        <v>83310211.5288</v>
+        <v>2149306</v>
       </c>
       <c r="D15" t="n">
-        <v>470719506.2083333</v>
+        <v>38823</v>
       </c>
       <c r="E15" t="n">
-        <v>1568.302256322125</v>
+        <v>2209.007</v>
       </c>
       <c r="F15" t="n">
-        <v>31.10074629166667</v>
+        <v>5.388297</v>
       </c>
       <c r="G15" t="n">
-        <v>29.60715916666667</v>
+        <v>15.03891</v>
       </c>
       <c r="H15" t="n">
-        <v>13.32159295454545</v>
+        <v>4.079457</v>
       </c>
       <c r="I15" t="n">
-        <v>59.00027681818182</v>
+        <v>39.22143</v>
       </c>
       <c r="J15" t="n">
-        <v>35.2782835</v>
+        <v>14.12866</v>
       </c>
       <c r="K15" t="n">
-        <v>167.0654287142857</v>
+        <v>11.78862</v>
       </c>
       <c r="L15" t="n">
-        <v>954.2403285714287</v>
+        <v>625.8274</v>
       </c>
       <c r="M15" t="n">
-        <v>73.55111304761905</v>
+        <v>14.28396</v>
       </c>
       <c r="N15" t="n">
-        <v>6684204.01</v>
+        <v>182863.2</v>
       </c>
       <c r="O15" t="n">
-        <v>13605.96915</v>
+        <v>1613.577</v>
       </c>
       <c r="P15" t="n">
-        <v>163.0530085</v>
+        <v>112.4737</v>
       </c>
       <c r="Q15" t="n">
-        <v>1653.977866</v>
+        <v>546.3324</v>
       </c>
       <c r="R15" t="n">
-        <v>127.66748875</v>
+        <v>26.53549</v>
       </c>
       <c r="S15" t="n">
-        <v>91.3482715</v>
+        <v>37.83339</v>
       </c>
       <c r="T15" t="n">
-        <v>81539.5255</v>
+        <v>2596.993</v>
       </c>
       <c r="U15" t="n">
-        <v>20964.6721285</v>
+        <v>77.1284</v>
       </c>
       <c r="V15" t="n">
-        <v>97.297777</v>
+        <v>33.28729</v>
       </c>
       <c r="W15" t="n">
-        <v>134.2013</v>
+        <v>111.4889</v>
       </c>
       <c r="X15" t="n">
-        <v>395.9836142105263</v>
+        <v>110.8909</v>
       </c>
       <c r="Y15" t="n">
-        <v>329.0149263157895</v>
+        <v>312.164</v>
       </c>
       <c r="Z15" t="n">
-        <v>351.0559888888889</v>
+        <v>343.487</v>
       </c>
       <c r="AA15" t="n">
-        <v>428.5550611111111</v>
+        <v>406.1602</v>
       </c>
       <c r="AB15" t="n">
-        <v>523.4791666666666</v>
+        <v>315.3383</v>
       </c>
       <c r="AC15" t="n">
-        <v>398.8346666666667</v>
+        <v>390.5696</v>
       </c>
       <c r="AD15" t="n">
-        <v>411.01375</v>
+        <v>349.632</v>
       </c>
       <c r="AE15" t="n">
-        <v>312.3104944444444</v>
+        <v>289.422</v>
       </c>
       <c r="AF15" t="n">
-        <v>437370.0216666667</v>
+        <v>51969.3</v>
       </c>
       <c r="AG15" t="n">
         <v>10</v>

</xml_diff>